<commit_message>
Finished soda rerun metadata
</commit_message>
<xml_diff>
--- a/scripts/projects/soda_rerun/meta_data.xlsx
+++ b/scripts/projects/soda_rerun/meta_data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="127">
   <si>
     <t>Sample</t>
   </si>
@@ -249,9 +249,6 @@
     <t>SS01</t>
   </si>
   <si>
-    <t>SS02</t>
-  </si>
-  <si>
     <t>SS12</t>
   </si>
   <si>
@@ -276,9 +273,6 @@
     <t>Sample_SS01</t>
   </si>
   <si>
-    <t>Sample_SS02</t>
-  </si>
-  <si>
     <t>Sample_SS10</t>
   </si>
   <si>
@@ -315,9 +309,6 @@
     <t>ss01</t>
   </si>
   <si>
-    <t>ss02</t>
-  </si>
-  <si>
     <t>ss10</t>
   </si>
   <si>
@@ -394,6 +385,21 @@
   </si>
   <si>
     <t>german</t>
+  </si>
+  <si>
+    <t>SS04</t>
+  </si>
+  <si>
+    <t>ss04</t>
+  </si>
+  <si>
+    <t>Sample_SS04</t>
+  </si>
+  <si>
+    <t>Sample remarks</t>
+  </si>
+  <si>
+    <t>This one is found in ILLUMITAG run 4, pool 4 instead.</t>
   </si>
 </sst>
 </file>
@@ -1252,7 +1258,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1521,6 +1527,18 @@
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="55">
@@ -1987,13 +2005,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BK11"/>
+  <dimension ref="A1:BL11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="V2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="P16" sqref="P16"/>
+      <selection pane="bottomRight" activeCell="Z13" sqref="Z13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2003,32 +2021,32 @@
     <col min="7" max="7" width="10.6640625" style="1" customWidth="1"/>
     <col min="16" max="16" width="15" customWidth="1"/>
     <col min="20" max="20" width="13.1640625" customWidth="1"/>
-    <col min="22" max="24" width="17.5" customWidth="1"/>
-    <col min="29" max="29" width="13.83203125" customWidth="1"/>
-    <col min="30" max="30" width="14.83203125" customWidth="1"/>
-    <col min="32" max="32" width="15.33203125" customWidth="1"/>
-    <col min="33" max="33" width="23.5" customWidth="1"/>
-    <col min="35" max="35" width="15.83203125" customWidth="1"/>
-    <col min="36" max="36" width="28.83203125" customWidth="1"/>
-    <col min="37" max="37" width="21" customWidth="1"/>
-    <col min="38" max="38" width="22.33203125" customWidth="1"/>
-    <col min="39" max="39" width="11" customWidth="1"/>
-    <col min="40" max="40" width="22.33203125" customWidth="1"/>
-    <col min="41" max="41" width="15.83203125" customWidth="1"/>
-    <col min="42" max="42" width="9.33203125" customWidth="1"/>
-    <col min="44" max="44" width="16" customWidth="1"/>
-    <col min="48" max="48" width="14.6640625" customWidth="1"/>
-    <col min="52" max="52" width="18.83203125" customWidth="1"/>
-    <col min="53" max="53" width="17.33203125" customWidth="1"/>
-    <col min="54" max="54" width="14.83203125" customWidth="1"/>
-    <col min="55" max="58" width="17.6640625" customWidth="1"/>
-    <col min="60" max="60" width="19" customWidth="1"/>
-    <col min="61" max="61" width="11.83203125" customWidth="1"/>
-    <col min="62" max="62" width="15.33203125" customWidth="1"/>
-    <col min="63" max="63" width="17.6640625" customWidth="1"/>
+    <col min="22" max="25" width="17.5" customWidth="1"/>
+    <col min="30" max="30" width="13.83203125" customWidth="1"/>
+    <col min="31" max="31" width="14.83203125" customWidth="1"/>
+    <col min="33" max="33" width="15.33203125" customWidth="1"/>
+    <col min="34" max="34" width="23.5" customWidth="1"/>
+    <col min="36" max="36" width="15.83203125" customWidth="1"/>
+    <col min="37" max="37" width="28.83203125" customWidth="1"/>
+    <col min="38" max="38" width="21" customWidth="1"/>
+    <col min="39" max="39" width="22.33203125" customWidth="1"/>
+    <col min="40" max="40" width="11" customWidth="1"/>
+    <col min="41" max="41" width="22.33203125" customWidth="1"/>
+    <col min="42" max="42" width="15.83203125" customWidth="1"/>
+    <col min="43" max="43" width="9.33203125" customWidth="1"/>
+    <col min="45" max="45" width="16" customWidth="1"/>
+    <col min="49" max="49" width="14.6640625" customWidth="1"/>
+    <col min="53" max="53" width="18.83203125" customWidth="1"/>
+    <col min="54" max="54" width="17.33203125" customWidth="1"/>
+    <col min="55" max="55" width="14.83203125" customWidth="1"/>
+    <col min="56" max="59" width="17.6640625" customWidth="1"/>
+    <col min="61" max="61" width="19" customWidth="1"/>
+    <col min="62" max="62" width="11.83203125" customWidth="1"/>
+    <col min="63" max="63" width="15.33203125" customWidth="1"/>
+    <col min="64" max="64" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:63" ht="31" thickTop="1">
+    <row r="1" spans="1:64" ht="31" thickTop="1">
       <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
@@ -2039,10 +2057,10 @@
         <v>5</v>
       </c>
       <c r="D1" s="57" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E1" s="57" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F1" s="78" t="s">
         <v>2</v>
@@ -2051,31 +2069,31 @@
         <v>1</v>
       </c>
       <c r="H1" s="57" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="I1" s="57" t="s">
+        <v>108</v>
+      </c>
+      <c r="J1" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="K1" s="61" t="s">
+        <v>110</v>
+      </c>
+      <c r="L1" s="59" t="s">
         <v>111</v>
       </c>
-      <c r="J1" s="57" t="s">
+      <c r="M1" s="72" t="s">
         <v>112</v>
       </c>
-      <c r="K1" s="61" t="s">
+      <c r="N1" s="72" t="s">
         <v>113</v>
-      </c>
-      <c r="L1" s="59" t="s">
-        <v>114</v>
-      </c>
-      <c r="M1" s="72" t="s">
-        <v>115</v>
-      </c>
-      <c r="N1" s="72" t="s">
-        <v>116</v>
       </c>
       <c r="O1" s="9" t="s">
         <v>3</v>
       </c>
       <c r="P1" s="9" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="S1" s="15" t="s">
         <v>9</v>
@@ -2093,174 +2111,177 @@
         <v>71</v>
       </c>
       <c r="X1" s="19" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="Y1" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="Z1" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="Z1" s="19" t="s">
+      <c r="AA1" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="AA1" s="19" t="s">
+      <c r="AB1" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="AB1" s="19" t="s">
+      <c r="AC1" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="AC1" s="19" t="s">
+      <c r="AD1" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="AD1" s="19" t="s">
+      <c r="AE1" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="AE1" s="19" t="s">
+      <c r="AF1" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="AF1" s="19" t="s">
+      <c r="AG1" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="AG1" s="19" t="s">
+      <c r="AH1" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="AH1" s="19" t="s">
+      <c r="AI1" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="AI1" s="19" t="s">
+      <c r="AJ1" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="AJ1" s="19" t="s">
+      <c r="AK1" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="AK1" s="19" t="s">
+      <c r="AL1" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="AL1" s="19" t="s">
+      <c r="AM1" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="AM1" s="19" t="s">
+      <c r="AN1" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="AN1" s="19" t="s">
+      <c r="AO1" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="AO1" s="19" t="s">
+      <c r="AP1" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="AP1" s="19" t="s">
+      <c r="AQ1" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="AQ1" s="19" t="s">
+      <c r="AR1" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="AR1" s="19" t="s">
+      <c r="AS1" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="AS1" s="19" t="s">
+      <c r="AT1" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="AT1" s="19" t="s">
+      <c r="AU1" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="AU1" s="19" t="s">
+      <c r="AV1" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="AV1" s="19" t="s">
+      <c r="AW1" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="AW1" s="19" t="s">
+      <c r="AX1" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="AX1" s="19" t="s">
+      <c r="AY1" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="AY1" s="19" t="s">
+      <c r="AZ1" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="AZ1" s="30" t="s">
+      <c r="BA1" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="BA1" s="30" t="s">
+      <c r="BB1" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="BB1" s="30" t="s">
+      <c r="BC1" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="BC1" s="30" t="s">
+      <c r="BD1" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="BD1" s="33" t="s">
+      <c r="BE1" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="BE1" s="33" t="s">
+      <c r="BF1" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="BF1" s="33" t="s">
+      <c r="BG1" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="BG1" s="31" t="s">
+      <c r="BH1" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="BH1" s="31" t="s">
+      <c r="BI1" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="BI1" s="31" t="s">
+      <c r="BJ1" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="BJ1" s="32" t="s">
+      <c r="BK1" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="BK1" s="68" t="s">
+      <c r="BL1" s="68" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:63" ht="16" customHeight="1" thickBot="1">
+    <row r="2" spans="1:64" ht="16" customHeight="1" thickBot="1">
       <c r="A2" s="4"/>
       <c r="B2" s="7"/>
       <c r="C2" s="8"/>
       <c r="D2" s="58" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E2" s="58" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F2" s="79" t="s">
         <v>4</v>
       </c>
       <c r="G2" s="58"/>
       <c r="H2" s="58" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="I2" s="58" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J2" s="58" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="K2" s="62" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="L2" s="60" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="M2" s="58" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="N2" s="58" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="O2" s="10" t="s">
         <v>7</v>
       </c>
       <c r="P2" s="10" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="S2" s="16" t="s">
         <v>74</v>
       </c>
       <c r="T2" s="22"/>
-      <c r="BK2" s="69"/>
+      <c r="BL2" s="69"/>
     </row>
-    <row r="3" spans="1:63" ht="16" customHeight="1" thickTop="1">
+    <row r="3" spans="1:64" ht="16" customHeight="1" thickTop="1">
       <c r="A3" s="2">
         <v>19</v>
       </c>
@@ -2278,8 +2299,8 @@
       <c r="G3" s="76">
         <v>9.6999999999999993</v>
       </c>
-      <c r="H3" s="73">
-        <v>16.7</v>
+      <c r="H3" s="99">
+        <v>16700</v>
       </c>
       <c r="I3" s="81"/>
       <c r="J3" s="81"/>
@@ -2289,7 +2310,7 @@
       <c r="N3" s="83"/>
       <c r="O3" s="84"/>
       <c r="P3" s="84" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="R3" s="14" t="s">
         <v>8</v>
@@ -2301,125 +2322,125 @@
         <v>13</v>
       </c>
       <c r="U3" t="s">
+        <v>82</v>
+      </c>
+      <c r="V3" t="s">
         <v>83</v>
       </c>
-      <c r="V3" t="s">
-        <v>84</v>
-      </c>
       <c r="W3" t="s">
+        <v>90</v>
+      </c>
+      <c r="X3" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z3" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="AA3" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="X3" t="s">
-        <v>120</v>
-      </c>
-      <c r="Y3" s="25" t="s">
-        <v>93</v>
-      </c>
-      <c r="Z3" s="25" t="s">
-        <v>94</v>
-      </c>
-      <c r="AA3" s="25"/>
       <c r="AB3" s="25"/>
       <c r="AC3" s="25"/>
       <c r="AD3" s="25"/>
-      <c r="AE3" s="26" t="s">
+      <c r="AE3" s="25"/>
+      <c r="AF3" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="AF3" s="27" t="s">
+      <c r="AG3" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="AG3" s="28" t="s">
+      <c r="AH3" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="AH3" s="26" t="s">
+      <c r="AI3" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="AI3" s="27" t="s">
+      <c r="AJ3" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="AJ3" s="29" t="s">
+      <c r="AK3" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="AK3" s="20" t="s">
+      <c r="AL3" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="AM3" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="AN3" s="21">
+        <v>7</v>
+      </c>
+      <c r="AO3" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="AL3" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="AM3" s="21">
-        <v>7</v>
-      </c>
-      <c r="AN3" s="24" t="s">
-        <v>97</v>
-      </c>
-      <c r="AO3" s="22" t="s">
+      <c r="AP3" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="AP3" s="24">
+      <c r="AQ3" s="24">
         <v>1</v>
       </c>
-      <c r="AQ3" t="s">
+      <c r="AR3" t="s">
         <v>46</v>
       </c>
-      <c r="AR3" t="s">
+      <c r="AS3" t="s">
         <v>47</v>
       </c>
-      <c r="AS3" t="s">
+      <c r="AT3" t="s">
         <v>48</v>
       </c>
-      <c r="AT3" s="23" t="s">
+      <c r="AU3" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="AU3" s="23" t="s">
+      <c r="AV3" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="AV3" s="23" t="s">
+      <c r="AW3" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="AW3" s="23" t="s">
-        <v>105</v>
-      </c>
-      <c r="AX3" s="23">
-        <v>125</v>
+      <c r="AX3" s="23" t="s">
+        <v>102</v>
       </c>
       <c r="AY3" s="23">
         <v>125</v>
       </c>
-      <c r="AZ3" s="23" t="s">
+      <c r="AZ3" s="23">
+        <v>125</v>
+      </c>
+      <c r="BA3" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="BA3" s="23" t="s">
+      <c r="BB3" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="BB3" s="23" t="s">
+      <c r="BC3" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="BC3" s="23" t="s">
+      <c r="BD3" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="BD3" s="66">
+      <c r="BE3" s="66">
         <v>41001</v>
       </c>
-      <c r="BE3" s="22">
+      <c r="BF3" s="22">
         <v>47.791389000000002</v>
       </c>
-      <c r="BF3" s="22">
+      <c r="BG3" s="22">
         <v>16.780556000000001</v>
       </c>
-      <c r="BG3" t="s">
-        <v>106</v>
-      </c>
       <c r="BH3" t="s">
-        <v>107</v>
-      </c>
-      <c r="BJ3" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="BI3" t="s">
+        <v>104</v>
+      </c>
+      <c r="BK3" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="BK3" s="70" t="s">
+      <c r="BL3" s="70" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:63" ht="15" customHeight="1">
+    <row r="4" spans="1:64" ht="15" customHeight="1">
       <c r="A4" s="3">
         <v>21</v>
       </c>
@@ -2435,8 +2456,8 @@
       <c r="G4" s="77">
         <v>10.15</v>
       </c>
-      <c r="H4" s="74">
-        <v>16</v>
+      <c r="H4" s="100">
+        <v>16000</v>
       </c>
       <c r="I4" s="86"/>
       <c r="J4" s="86"/>
@@ -2446,137 +2467,137 @@
       <c r="N4" s="88"/>
       <c r="O4" s="89"/>
       <c r="P4" s="89" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="R4" s="14" t="s">
         <v>8</v>
       </c>
       <c r="S4" s="18" t="s">
-        <v>76</v>
+        <v>122</v>
       </c>
       <c r="T4" s="22" t="s">
         <v>13</v>
       </c>
       <c r="U4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="V4" t="s">
-        <v>85</v>
+        <v>124</v>
       </c>
       <c r="W4" t="s">
+        <v>90</v>
+      </c>
+      <c r="X4" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z4" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="AA4" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="X4" t="s">
-        <v>120</v>
-      </c>
-      <c r="Y4" s="25" t="s">
-        <v>93</v>
-      </c>
-      <c r="Z4" s="25" t="s">
-        <v>94</v>
-      </c>
-      <c r="AA4" s="25"/>
       <c r="AB4" s="25"/>
       <c r="AC4" s="25"/>
       <c r="AD4" s="25"/>
-      <c r="AE4" s="26" t="s">
+      <c r="AE4" s="25"/>
+      <c r="AF4" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="AF4" s="27" t="s">
+      <c r="AG4" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="AG4" s="28" t="s">
+      <c r="AH4" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="AH4" s="26" t="s">
+      <c r="AI4" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="AI4" s="27" t="s">
+      <c r="AJ4" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="AJ4" s="29" t="s">
+      <c r="AK4" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="AK4" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="AL4" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="AM4" s="21">
+      <c r="AL4" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="AM4" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="AN4" s="21">
         <v>7</v>
       </c>
-      <c r="AN4" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="AO4" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="AP4" s="24">
+      <c r="AO4" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="AP4" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="AQ4" s="24">
         <v>2</v>
       </c>
-      <c r="AQ4" t="s">
+      <c r="AR4" t="s">
         <v>46</v>
       </c>
-      <c r="AR4" t="s">
+      <c r="AS4" t="s">
         <v>47</v>
       </c>
-      <c r="AS4" t="s">
+      <c r="AT4" t="s">
         <v>48</v>
       </c>
-      <c r="AT4" s="23" t="s">
+      <c r="AU4" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="AU4" s="23" t="s">
+      <c r="AV4" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="AV4" s="23" t="s">
+      <c r="AW4" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="AW4" s="23" t="s">
-        <v>105</v>
-      </c>
-      <c r="AX4" s="23">
-        <v>125</v>
+      <c r="AX4" s="23" t="s">
+        <v>102</v>
       </c>
       <c r="AY4" s="23">
         <v>125</v>
       </c>
-      <c r="AZ4" s="23" t="s">
+      <c r="AZ4" s="23">
+        <v>125</v>
+      </c>
+      <c r="BA4" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="BA4" s="23" t="s">
+      <c r="BB4" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="BB4" s="23" t="s">
+      <c r="BC4" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="BC4" s="23" t="s">
+      <c r="BD4" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="BD4" s="66">
+      <c r="BE4" s="66">
         <v>41043</v>
       </c>
-      <c r="BE4" s="22">
+      <c r="BF4" s="22">
         <v>47.791389000000002</v>
       </c>
-      <c r="BF4" s="22">
+      <c r="BG4" s="22">
         <v>16.780556000000001</v>
       </c>
-      <c r="BG4" t="s">
-        <v>106</v>
-      </c>
       <c r="BH4" t="s">
-        <v>107</v>
-      </c>
-      <c r="BJ4" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="BI4" t="s">
+        <v>104</v>
+      </c>
+      <c r="BK4" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="BK4" s="70" t="s">
+      <c r="BL4" s="70" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:63" ht="15" customHeight="1">
+    <row r="5" spans="1:64" ht="15" customHeight="1">
       <c r="A5" s="3">
         <v>23</v>
       </c>
@@ -2592,8 +2613,8 @@
       <c r="G5" s="77">
         <v>10.199999999999999</v>
       </c>
-      <c r="H5" s="74">
-        <v>7.9</v>
+      <c r="H5" s="100">
+        <v>7900</v>
       </c>
       <c r="I5" s="86"/>
       <c r="J5" s="86"/>
@@ -2603,137 +2624,137 @@
       <c r="N5" s="88"/>
       <c r="O5" s="89"/>
       <c r="P5" s="89" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="R5" s="14" t="s">
         <v>8</v>
       </c>
       <c r="S5" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="T5" s="22" t="s">
         <v>13</v>
       </c>
       <c r="U5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="V5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="W5" t="s">
+        <v>90</v>
+      </c>
+      <c r="X5" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z5" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="AA5" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="X5" t="s">
-        <v>120</v>
-      </c>
-      <c r="Y5" s="25" t="s">
-        <v>93</v>
-      </c>
-      <c r="Z5" s="25" t="s">
-        <v>94</v>
-      </c>
-      <c r="AA5" s="25"/>
       <c r="AB5" s="25"/>
       <c r="AC5" s="25"/>
       <c r="AD5" s="25"/>
-      <c r="AE5" s="26" t="s">
+      <c r="AE5" s="25"/>
+      <c r="AF5" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="AF5" s="27" t="s">
+      <c r="AG5" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="AG5" s="28" t="s">
+      <c r="AH5" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="AH5" s="26" t="s">
+      <c r="AI5" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="AI5" s="27" t="s">
+      <c r="AJ5" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="AJ5" s="29" t="s">
+      <c r="AK5" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="AK5" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="AL5" s="21" t="s">
+      <c r="AL5" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="AM5" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="AN5" s="21">
+        <v>7</v>
+      </c>
+      <c r="AO5" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="AM5" s="21">
-        <v>7</v>
-      </c>
-      <c r="AN5" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="AO5" s="22" t="s">
-        <v>82</v>
-      </c>
-      <c r="AP5" s="24">
+      <c r="AP5" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="AQ5" s="24">
         <v>3</v>
       </c>
-      <c r="AQ5" t="s">
+      <c r="AR5" t="s">
         <v>46</v>
       </c>
-      <c r="AR5" t="s">
+      <c r="AS5" t="s">
         <v>47</v>
       </c>
-      <c r="AS5" t="s">
+      <c r="AT5" t="s">
         <v>48</v>
       </c>
-      <c r="AT5" s="23" t="s">
+      <c r="AU5" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="AU5" s="23" t="s">
+      <c r="AV5" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="AV5" s="23" t="s">
+      <c r="AW5" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="AW5" s="23" t="s">
-        <v>105</v>
-      </c>
-      <c r="AX5" s="23">
-        <v>125</v>
+      <c r="AX5" s="23" t="s">
+        <v>102</v>
       </c>
       <c r="AY5" s="23">
         <v>125</v>
       </c>
-      <c r="AZ5" s="23" t="s">
+      <c r="AZ5" s="23">
+        <v>125</v>
+      </c>
+      <c r="BA5" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="BA5" s="23" t="s">
+      <c r="BB5" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="BB5" s="23" t="s">
+      <c r="BC5" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="BC5" s="23" t="s">
+      <c r="BD5" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="BD5" s="66">
+      <c r="BE5" s="66">
         <v>41127</v>
       </c>
-      <c r="BE5" s="22">
+      <c r="BF5" s="22">
         <v>47.791389000000002</v>
       </c>
-      <c r="BF5" s="22">
+      <c r="BG5" s="22">
         <v>16.780556000000001</v>
       </c>
-      <c r="BG5" t="s">
-        <v>106</v>
-      </c>
       <c r="BH5" t="s">
-        <v>107</v>
-      </c>
-      <c r="BJ5" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="BI5" t="s">
+        <v>104</v>
+      </c>
+      <c r="BK5" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="BK5" s="70" t="s">
+      <c r="BL5" s="70" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:63" ht="15" customHeight="1" thickBot="1">
+    <row r="6" spans="1:64" ht="15" customHeight="1" thickBot="1">
       <c r="A6" s="3">
         <v>25</v>
       </c>
@@ -2749,8 +2770,8 @@
       <c r="G6" s="85">
         <v>10.26</v>
       </c>
-      <c r="H6" s="86">
-        <v>19.3</v>
+      <c r="H6" s="101">
+        <v>19300</v>
       </c>
       <c r="I6" s="86">
         <v>10569</v>
@@ -2772,137 +2793,137 @@
       </c>
       <c r="O6" s="89"/>
       <c r="P6" s="89" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="R6" s="14" t="s">
         <v>8</v>
       </c>
       <c r="S6" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="T6" s="22" t="s">
         <v>13</v>
       </c>
       <c r="U6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="V6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="W6" t="s">
+        <v>90</v>
+      </c>
+      <c r="X6" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z6" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="AA6" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="X6" t="s">
-        <v>120</v>
-      </c>
-      <c r="Y6" s="25" t="s">
-        <v>93</v>
-      </c>
-      <c r="Z6" s="25" t="s">
-        <v>94</v>
-      </c>
-      <c r="AA6" s="25"/>
       <c r="AB6" s="25"/>
       <c r="AC6" s="25"/>
       <c r="AD6" s="25"/>
-      <c r="AE6" s="26" t="s">
+      <c r="AE6" s="25"/>
+      <c r="AF6" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="AF6" s="27" t="s">
+      <c r="AG6" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="AG6" s="28" t="s">
+      <c r="AH6" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="AH6" s="26" t="s">
+      <c r="AI6" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="AI6" s="27" t="s">
+      <c r="AJ6" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="AJ6" s="29" t="s">
+      <c r="AK6" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="AK6" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="AL6" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="AM6" s="21">
+      <c r="AL6" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="AM6" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="AN6" s="21">
         <v>7</v>
       </c>
-      <c r="AN6" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="AO6" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="AP6" s="24">
+      <c r="AO6" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="AP6" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="AQ6" s="24">
         <v>4</v>
       </c>
-      <c r="AQ6" t="s">
+      <c r="AR6" t="s">
         <v>46</v>
       </c>
-      <c r="AR6" t="s">
+      <c r="AS6" t="s">
         <v>47</v>
       </c>
-      <c r="AS6" t="s">
+      <c r="AT6" t="s">
         <v>48</v>
       </c>
-      <c r="AT6" s="23" t="s">
+      <c r="AU6" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="AU6" s="23" t="s">
+      <c r="AV6" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="AV6" s="23" t="s">
+      <c r="AW6" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="AW6" s="23" t="s">
-        <v>105</v>
-      </c>
-      <c r="AX6" s="23">
-        <v>125</v>
+      <c r="AX6" s="23" t="s">
+        <v>102</v>
       </c>
       <c r="AY6" s="23">
         <v>125</v>
       </c>
-      <c r="AZ6" s="23" t="s">
+      <c r="AZ6" s="23">
+        <v>125</v>
+      </c>
+      <c r="BA6" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="BA6" s="23" t="s">
+      <c r="BB6" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="BB6" s="23" t="s">
+      <c r="BC6" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="BC6" s="23" t="s">
+      <c r="BD6" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="BD6" s="66">
+      <c r="BE6" s="66">
         <v>41162</v>
       </c>
-      <c r="BE6" s="22">
+      <c r="BF6" s="22">
         <v>47.791389000000002</v>
       </c>
-      <c r="BF6" s="22">
+      <c r="BG6" s="22">
         <v>16.780556000000001</v>
       </c>
-      <c r="BG6" t="s">
-        <v>106</v>
-      </c>
       <c r="BH6" t="s">
-        <v>107</v>
-      </c>
-      <c r="BJ6" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="BI6" t="s">
+        <v>104</v>
+      </c>
+      <c r="BK6" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="BK6" s="70" t="s">
+      <c r="BL6" s="70" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:63" ht="16" customHeight="1" thickTop="1">
+    <row r="7" spans="1:64" ht="16" customHeight="1" thickTop="1">
       <c r="A7" s="2">
         <v>35</v>
       </c>
@@ -2924,8 +2945,8 @@
       <c r="G7" s="85">
         <v>9.8000000000000007</v>
       </c>
-      <c r="H7" s="86">
-        <v>13.2</v>
+      <c r="H7" s="101">
+        <v>13200</v>
       </c>
       <c r="I7" s="86">
         <v>3321</v>
@@ -2949,139 +2970,139 @@
         <v>329062500</v>
       </c>
       <c r="P7" s="84" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="Q7" s="34"/>
       <c r="R7" s="14" t="s">
         <v>8</v>
       </c>
       <c r="S7" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="T7" s="35" t="s">
         <v>13</v>
       </c>
       <c r="U7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="V7" s="34" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="W7" t="s">
+        <v>90</v>
+      </c>
+      <c r="X7" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z7" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="AA7" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="X7" t="s">
-        <v>120</v>
-      </c>
-      <c r="Y7" s="25" t="s">
-        <v>93</v>
-      </c>
-      <c r="Z7" s="25" t="s">
-        <v>94</v>
-      </c>
-      <c r="AA7" s="36"/>
       <c r="AB7" s="36"/>
       <c r="AC7" s="36"/>
       <c r="AD7" s="36"/>
-      <c r="AE7" s="37" t="s">
+      <c r="AE7" s="36"/>
+      <c r="AF7" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="AF7" s="38" t="s">
+      <c r="AG7" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="AG7" s="39" t="s">
+      <c r="AH7" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="AH7" s="37" t="s">
+      <c r="AI7" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="AI7" s="38" t="s">
+      <c r="AJ7" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="AJ7" s="40" t="s">
+      <c r="AK7" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="AK7" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="AL7" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="AM7" s="21">
+      <c r="AL7" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="AM7" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="AN7" s="21">
         <v>7</v>
       </c>
-      <c r="AN7" s="41" t="s">
-        <v>101</v>
-      </c>
-      <c r="AO7" s="35" t="s">
-        <v>78</v>
-      </c>
-      <c r="AP7" s="41">
-        <v>1</v>
-      </c>
-      <c r="AQ7" s="34" t="s">
+      <c r="AO7" s="41" t="s">
+        <v>98</v>
+      </c>
+      <c r="AP7" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="AQ7" s="41">
+        <v>5</v>
+      </c>
+      <c r="AR7" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="AR7" s="34" t="s">
+      <c r="AS7" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="AS7" s="34" t="s">
+      <c r="AT7" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="AT7" s="42" t="s">
+      <c r="AU7" s="42" t="s">
         <v>49</v>
       </c>
-      <c r="AU7" s="42" t="s">
+      <c r="AV7" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="AV7" s="42" t="s">
+      <c r="AW7" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="AW7" s="23" t="s">
-        <v>105</v>
-      </c>
-      <c r="AX7" s="42">
-        <v>125</v>
+      <c r="AX7" s="23" t="s">
+        <v>102</v>
       </c>
       <c r="AY7" s="42">
         <v>125</v>
       </c>
-      <c r="AZ7" s="42" t="s">
+      <c r="AZ7" s="42">
+        <v>125</v>
+      </c>
+      <c r="BA7" s="42" t="s">
         <v>63</v>
       </c>
-      <c r="BA7" s="42" t="s">
+      <c r="BB7" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="BB7" s="42" t="s">
+      <c r="BC7" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="BC7" s="42" t="s">
+      <c r="BD7" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="BD7" s="66">
+      <c r="BE7" s="66">
         <v>41001</v>
       </c>
-      <c r="BE7" s="35">
+      <c r="BF7" s="35">
         <v>47.768056000000001</v>
       </c>
-      <c r="BF7" s="35">
+      <c r="BG7" s="35">
         <v>16.780833000000001</v>
       </c>
-      <c r="BG7" t="s">
-        <v>106</v>
-      </c>
       <c r="BH7" t="s">
-        <v>107</v>
-      </c>
-      <c r="BI7" s="34"/>
-      <c r="BJ7" s="42" t="s">
+        <v>103</v>
+      </c>
+      <c r="BI7" t="s">
+        <v>104</v>
+      </c>
+      <c r="BJ7" s="34"/>
+      <c r="BK7" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="BK7" s="70" t="s">
+      <c r="BL7" s="70" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:63" ht="15" customHeight="1">
+    <row r="8" spans="1:64" ht="15" customHeight="1">
       <c r="A8" s="3">
         <v>37</v>
       </c>
@@ -3101,8 +3122,8 @@
       <c r="G8" s="85">
         <v>10.1</v>
       </c>
-      <c r="H8" s="86">
-        <v>14.3</v>
+      <c r="H8" s="101">
+        <v>14300</v>
       </c>
       <c r="I8" s="86">
         <v>1059</v>
@@ -3126,139 +3147,139 @@
         <v>281812500</v>
       </c>
       <c r="P8" s="89" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="Q8" s="34"/>
       <c r="R8" s="14" t="s">
         <v>8</v>
       </c>
       <c r="S8" s="18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="T8" s="35" t="s">
         <v>13</v>
       </c>
       <c r="U8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="V8" s="34" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="W8" t="s">
+        <v>90</v>
+      </c>
+      <c r="X8" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z8" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="AA8" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="X8" t="s">
-        <v>120</v>
-      </c>
-      <c r="Y8" s="25" t="s">
-        <v>93</v>
-      </c>
-      <c r="Z8" s="25" t="s">
-        <v>94</v>
-      </c>
-      <c r="AA8" s="36"/>
       <c r="AB8" s="36"/>
       <c r="AC8" s="36"/>
       <c r="AD8" s="36"/>
-      <c r="AE8" s="37" t="s">
+      <c r="AE8" s="36"/>
+      <c r="AF8" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="AF8" s="38" t="s">
+      <c r="AG8" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="AG8" s="39" t="s">
+      <c r="AH8" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="AH8" s="37" t="s">
+      <c r="AI8" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="AI8" s="38" t="s">
+      <c r="AJ8" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="AJ8" s="40" t="s">
+      <c r="AK8" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="AK8" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="AL8" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="AM8" s="21">
+      <c r="AL8" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="AM8" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="AN8" s="21">
         <v>7</v>
       </c>
-      <c r="AN8" s="41" t="s">
+      <c r="AO8" s="41" t="s">
+        <v>99</v>
+      </c>
+      <c r="AP8" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="AQ8" s="41">
+        <v>6</v>
+      </c>
+      <c r="AR8" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="AS8" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="AT8" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="AU8" s="42" t="s">
+        <v>49</v>
+      </c>
+      <c r="AV8" s="42" t="s">
+        <v>50</v>
+      </c>
+      <c r="AW8" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="AX8" s="23" t="s">
         <v>102</v>
-      </c>
-      <c r="AO8" s="35" t="s">
-        <v>79</v>
-      </c>
-      <c r="AP8" s="41">
-        <v>2</v>
-      </c>
-      <c r="AQ8" s="34" t="s">
-        <v>46</v>
-      </c>
-      <c r="AR8" s="34" t="s">
-        <v>47</v>
-      </c>
-      <c r="AS8" s="34" t="s">
-        <v>48</v>
-      </c>
-      <c r="AT8" s="42" t="s">
-        <v>49</v>
-      </c>
-      <c r="AU8" s="42" t="s">
-        <v>50</v>
-      </c>
-      <c r="AV8" s="42" t="s">
-        <v>51</v>
-      </c>
-      <c r="AW8" s="23" t="s">
-        <v>105</v>
-      </c>
-      <c r="AX8" s="42">
-        <v>125</v>
       </c>
       <c r="AY8" s="42">
         <v>125</v>
       </c>
-      <c r="AZ8" s="42" t="s">
+      <c r="AZ8" s="42">
+        <v>125</v>
+      </c>
+      <c r="BA8" s="42" t="s">
         <v>63</v>
       </c>
-      <c r="BA8" s="42" t="s">
+      <c r="BB8" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="BB8" s="42" t="s">
+      <c r="BC8" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="BC8" s="42" t="s">
+      <c r="BD8" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="BD8" s="66">
+      <c r="BE8" s="66">
         <v>41015</v>
       </c>
-      <c r="BE8" s="35">
+      <c r="BF8" s="35">
         <v>47.768056000000001</v>
       </c>
-      <c r="BF8" s="35">
+      <c r="BG8" s="35">
         <v>16.780833000000001</v>
       </c>
-      <c r="BG8" t="s">
-        <v>106</v>
-      </c>
       <c r="BH8" t="s">
-        <v>107</v>
-      </c>
-      <c r="BI8" s="34"/>
-      <c r="BJ8" s="42" t="s">
+        <v>103</v>
+      </c>
+      <c r="BI8" t="s">
+        <v>104</v>
+      </c>
+      <c r="BJ8" s="34"/>
+      <c r="BK8" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="BK8" s="70" t="s">
+      <c r="BL8" s="70" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:63" ht="15" customHeight="1">
+    <row r="9" spans="1:64" ht="15" customHeight="1">
       <c r="A9" s="3">
         <v>39</v>
       </c>
@@ -3278,8 +3299,8 @@
       <c r="G9" s="85">
         <v>10.16</v>
       </c>
-      <c r="H9" s="86">
-        <v>35.700000000000003</v>
+      <c r="H9" s="101">
+        <v>35700</v>
       </c>
       <c r="I9" s="86">
         <v>5323</v>
@@ -3303,139 +3324,139 @@
         <v>81000000</v>
       </c>
       <c r="P9" s="89" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="Q9" s="34"/>
       <c r="R9" s="14" t="s">
         <v>8</v>
       </c>
       <c r="S9" s="18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="T9" s="35" t="s">
         <v>13</v>
       </c>
       <c r="U9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="V9" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="W9" t="s">
         <v>90</v>
       </c>
-      <c r="W9" t="s">
+      <c r="X9" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z9" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="AA9" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="X9" t="s">
-        <v>120</v>
-      </c>
-      <c r="Y9" s="25" t="s">
-        <v>93</v>
-      </c>
-      <c r="Z9" s="25" t="s">
-        <v>94</v>
-      </c>
-      <c r="AA9" s="36"/>
       <c r="AB9" s="36"/>
       <c r="AC9" s="36"/>
       <c r="AD9" s="36"/>
-      <c r="AE9" s="37" t="s">
+      <c r="AE9" s="36"/>
+      <c r="AF9" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="AF9" s="38" t="s">
+      <c r="AG9" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="AG9" s="39" t="s">
+      <c r="AH9" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="AH9" s="37" t="s">
+      <c r="AI9" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="AI9" s="38" t="s">
+      <c r="AJ9" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="AJ9" s="40" t="s">
+      <c r="AK9" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="AK9" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="AL9" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="AM9" s="21">
+      <c r="AL9" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="AM9" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="AN9" s="21">
         <v>7</v>
       </c>
-      <c r="AN9" s="41" t="s">
-        <v>103</v>
-      </c>
-      <c r="AO9" s="35" t="s">
-        <v>80</v>
-      </c>
-      <c r="AP9" s="41">
-        <v>3</v>
-      </c>
-      <c r="AQ9" s="34" t="s">
+      <c r="AO9" s="41" t="s">
+        <v>100</v>
+      </c>
+      <c r="AP9" s="35" t="s">
+        <v>79</v>
+      </c>
+      <c r="AQ9" s="41">
+        <v>7</v>
+      </c>
+      <c r="AR9" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="AR9" s="34" t="s">
+      <c r="AS9" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="AS9" s="34" t="s">
+      <c r="AT9" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="AT9" s="42" t="s">
+      <c r="AU9" s="42" t="s">
         <v>49</v>
       </c>
-      <c r="AU9" s="42" t="s">
+      <c r="AV9" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="AV9" s="42" t="s">
+      <c r="AW9" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="AW9" s="23" t="s">
-        <v>105</v>
-      </c>
-      <c r="AX9" s="42">
-        <v>125</v>
+      <c r="AX9" s="23" t="s">
+        <v>102</v>
       </c>
       <c r="AY9" s="42">
         <v>125</v>
       </c>
-      <c r="AZ9" s="42" t="s">
+      <c r="AZ9" s="42">
+        <v>125</v>
+      </c>
+      <c r="BA9" s="42" t="s">
         <v>63</v>
       </c>
-      <c r="BA9" s="42" t="s">
+      <c r="BB9" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="BB9" s="42" t="s">
+      <c r="BC9" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="BC9" s="42" t="s">
+      <c r="BD9" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="BD9" s="66">
+      <c r="BE9" s="66">
         <v>41162</v>
       </c>
-      <c r="BE9" s="35">
+      <c r="BF9" s="35">
         <v>47.768056000000001</v>
       </c>
-      <c r="BF9" s="35">
+      <c r="BG9" s="35">
         <v>16.780833000000001</v>
       </c>
-      <c r="BG9" t="s">
-        <v>106</v>
-      </c>
       <c r="BH9" t="s">
-        <v>107</v>
-      </c>
-      <c r="BI9" s="34"/>
-      <c r="BJ9" s="42" t="s">
+        <v>103</v>
+      </c>
+      <c r="BI9" t="s">
+        <v>104</v>
+      </c>
+      <c r="BJ9" s="34"/>
+      <c r="BK9" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="BK9" s="70" t="s">
+      <c r="BL9" s="70" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:63" ht="15" customHeight="1" thickBot="1">
+    <row r="10" spans="1:64" ht="15" customHeight="1" thickBot="1">
       <c r="A10" s="3">
         <v>41</v>
       </c>
@@ -3444,184 +3465,177 @@
         <v>24</v>
       </c>
       <c r="D10" s="92">
-        <v>600.00000000000045</v>
+        <v>143.99999999999969</v>
       </c>
       <c r="E10" s="92">
-        <v>9.0704999999999991</v>
+        <v>22.957250000000002</v>
       </c>
       <c r="F10" s="93">
-        <v>9.1</v>
+        <v>1.4</v>
       </c>
       <c r="G10" s="94">
-        <v>9.26</v>
-      </c>
-      <c r="H10" s="92">
-        <v>0.4</v>
-      </c>
-      <c r="I10" s="92">
-        <v>201</v>
-      </c>
-      <c r="J10" s="92">
-        <v>138</v>
-      </c>
-      <c r="K10" s="95">
-        <v>370</v>
-      </c>
-      <c r="L10" s="96">
-        <v>23</v>
-      </c>
+        <v>8.9</v>
+      </c>
+      <c r="H10" s="102">
+        <v>1900</v>
+      </c>
+      <c r="I10" s="92"/>
+      <c r="J10" s="92"/>
+      <c r="K10" s="95"/>
+      <c r="L10" s="96"/>
       <c r="M10" s="97">
-        <v>540</v>
+        <v>240</v>
       </c>
       <c r="N10" s="97">
-        <v>46.5</v>
-      </c>
-      <c r="O10" s="98">
-        <v>38070000</v>
-      </c>
+        <v>31.4</v>
+      </c>
+      <c r="O10" s="98"/>
       <c r="P10" s="98" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="Q10" s="44"/>
       <c r="R10" s="45" t="s">
         <v>8</v>
       </c>
       <c r="S10" s="46" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="T10" s="47" t="s">
         <v>13</v>
       </c>
       <c r="U10" s="44" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="V10" s="44" t="s">
+        <v>89</v>
+      </c>
+      <c r="W10" s="44" t="s">
+        <v>90</v>
+      </c>
+      <c r="X10" s="44" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y10" s="44" t="s">
+        <v>126</v>
+      </c>
+      <c r="Z10" s="48" t="s">
         <v>91</v>
       </c>
-      <c r="W10" s="44" t="s">
+      <c r="AA10" s="48" t="s">
         <v>92</v>
       </c>
-      <c r="X10" s="44" t="s">
-        <v>120</v>
-      </c>
-      <c r="Y10" s="48" t="s">
-        <v>93</v>
-      </c>
-      <c r="Z10" s="48" t="s">
-        <v>94</v>
-      </c>
-      <c r="AA10" s="48"/>
       <c r="AB10" s="48"/>
       <c r="AC10" s="48"/>
       <c r="AD10" s="48"/>
-      <c r="AE10" s="49" t="s">
+      <c r="AE10" s="48"/>
+      <c r="AF10" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="AF10" s="50" t="s">
+      <c r="AG10" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="AG10" s="51" t="s">
+      <c r="AH10" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="AH10" s="49" t="s">
+      <c r="AI10" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="AI10" s="50" t="s">
+      <c r="AJ10" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="AJ10" s="52" t="s">
+      <c r="AK10" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="AK10" s="53" t="s">
-        <v>95</v>
-      </c>
-      <c r="AL10" s="44" t="s">
-        <v>96</v>
-      </c>
-      <c r="AM10" s="54">
+      <c r="AL10" s="53" t="s">
+        <v>93</v>
+      </c>
+      <c r="AM10" s="44" t="s">
+        <v>94</v>
+      </c>
+      <c r="AN10" s="54">
         <v>7</v>
       </c>
-      <c r="AN10" s="55" t="s">
-        <v>104</v>
-      </c>
-      <c r="AO10" s="47" t="s">
-        <v>81</v>
-      </c>
-      <c r="AP10" s="55">
-        <v>4</v>
-      </c>
-      <c r="AQ10" s="44" t="s">
+      <c r="AO10" s="55" t="s">
+        <v>101</v>
+      </c>
+      <c r="AP10" s="47" t="s">
+        <v>80</v>
+      </c>
+      <c r="AQ10" s="55">
+        <v>8</v>
+      </c>
+      <c r="AR10" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="AR10" s="44" t="s">
+      <c r="AS10" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="AS10" s="44" t="s">
+      <c r="AT10" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="AT10" s="56" t="s">
+      <c r="AU10" s="56" t="s">
         <v>49</v>
       </c>
-      <c r="AU10" s="56" t="s">
+      <c r="AV10" s="56" t="s">
         <v>50</v>
       </c>
-      <c r="AV10" s="56" t="s">
+      <c r="AW10" s="56" t="s">
         <v>51</v>
       </c>
-      <c r="AW10" s="56" t="s">
-        <v>105</v>
-      </c>
-      <c r="AX10" s="56">
-        <v>125</v>
+      <c r="AX10" s="56" t="s">
+        <v>102</v>
       </c>
       <c r="AY10" s="56">
         <v>125</v>
       </c>
-      <c r="AZ10" s="56" t="s">
+      <c r="AZ10" s="56">
+        <v>125</v>
+      </c>
+      <c r="BA10" s="56" t="s">
         <v>63</v>
       </c>
-      <c r="BA10" s="56" t="s">
+      <c r="BB10" s="56" t="s">
         <v>64</v>
       </c>
-      <c r="BB10" s="56" t="s">
+      <c r="BC10" s="56" t="s">
         <v>66</v>
       </c>
-      <c r="BC10" s="56" t="s">
+      <c r="BD10" s="56" t="s">
         <v>65</v>
       </c>
-      <c r="BD10" s="67">
-        <v>41218</v>
-      </c>
-      <c r="BE10" s="47">
+      <c r="BE10" s="67">
+        <v>41309</v>
+      </c>
+      <c r="BF10" s="47">
         <v>47.768056000000001</v>
       </c>
-      <c r="BF10" s="47">
+      <c r="BG10" s="47">
         <v>16.780833000000001</v>
       </c>
-      <c r="BG10" s="44" t="s">
-        <v>106</v>
-      </c>
       <c r="BH10" s="44" t="s">
-        <v>107</v>
-      </c>
-      <c r="BI10" s="44"/>
-      <c r="BJ10" s="56" t="s">
+        <v>103</v>
+      </c>
+      <c r="BI10" s="44" t="s">
+        <v>104</v>
+      </c>
+      <c r="BJ10" s="44"/>
+      <c r="BK10" s="56" t="s">
         <v>61</v>
       </c>
-      <c r="BK10" s="71" t="s">
+      <c r="BL10" s="71" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:63" ht="16" thickTop="1"/>
+    <row r="11" spans="1:64" ht="16" thickTop="1"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B3:B6"/>
     <mergeCell ref="B7:B10"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
-  <conditionalFormatting sqref="AA1:AB1">
+  <conditionalFormatting sqref="AB1:AC1">
     <cfRule type="containsBlanks" dxfId="0" priority="1" stopIfTrue="1">
-      <formula>LEN(TRIM(AA1))=0</formula>
+      <formula>LEN(TRIM(AB1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update read number and md5 hash soda_rerun
</commit_message>
<xml_diff>
--- a/scripts/projects/soda_rerun/meta_data.xlsx
+++ b/scripts/projects/soda_rerun/meta_data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="143">
   <si>
     <t>Sample</t>
   </si>
@@ -400,6 +400,54 @@
   </si>
   <si>
     <t>This one is found in ILLUMITAG run 4, pool 4 instead.</t>
+  </si>
+  <si>
+    <t>a7b04c567045ef4ef8d3838cffb4d5a9</t>
+  </si>
+  <si>
+    <t>aab80aef28c4e1b0b971cb84af62d41b</t>
+  </si>
+  <si>
+    <t>307e8b93e6141c5e1148331562142a68</t>
+  </si>
+  <si>
+    <t>dbd0c75cfd24bdb2271270c51be9b801</t>
+  </si>
+  <si>
+    <t>1cba9f85ccfa9bb083798b960143a79a</t>
+  </si>
+  <si>
+    <t>74c4f06936290d48d8ebcf99def294e6</t>
+  </si>
+  <si>
+    <t>55fd26f0c0e3964415ea8ae83a699454</t>
+  </si>
+  <si>
+    <t>1d6470067b9aa22d7e0b2b70d9033737</t>
+  </si>
+  <si>
+    <t>12c9fc0cdae4d667083c7f35fa7585b5</t>
+  </si>
+  <si>
+    <t>5ab4dbfbf98d4f38febc320ad309f455</t>
+  </si>
+  <si>
+    <t>df41ab47eee41cd52303fb82e4dfc446</t>
+  </si>
+  <si>
+    <t>50b3eed03ca51dad6a874c577c1a1913</t>
+  </si>
+  <si>
+    <t>23cd46ecc5b984f862ad8867bb8d1b92</t>
+  </si>
+  <si>
+    <t>a6b5acac07e4e09c4a64bd23641cf87a</t>
+  </si>
+  <si>
+    <t>626c5cb199a26a6c20a8b34fd3ada4ac</t>
+  </si>
+  <si>
+    <t>1be86e35b31b69037545bbf7417e8811</t>
   </si>
 </sst>
 </file>
@@ -409,7 +457,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
-    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="17" x14ac:knownFonts="1">
     <font>
@@ -1093,7 +1141,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="55">
+  <cellStyleXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1168,6 +1216,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1424,15 +1478,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1462,7 +1507,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1540,8 +1585,17 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="55">
+  <cellStyles count="57">
     <cellStyle name="Excel Built-in Normal" xfId="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -1582,6 +1636,7 @@
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
@@ -1596,6 +1651,7 @@
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="1">
@@ -2011,7 +2067,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="V2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Z13" sqref="Z13"/>
+      <selection pane="bottomRight" activeCell="AB15" sqref="AB15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2062,10 +2118,10 @@
       <c r="E1" s="57" t="s">
         <v>106</v>
       </c>
-      <c r="F1" s="78" t="s">
+      <c r="F1" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="75" t="s">
+      <c r="G1" s="72" t="s">
         <v>1</v>
       </c>
       <c r="H1" s="57" t="s">
@@ -2083,10 +2139,10 @@
       <c r="L1" s="59" t="s">
         <v>111</v>
       </c>
-      <c r="M1" s="72" t="s">
+      <c r="M1" s="69" t="s">
         <v>112</v>
       </c>
-      <c r="N1" s="72" t="s">
+      <c r="N1" s="69" t="s">
         <v>113</v>
       </c>
       <c r="O1" s="9" t="s">
@@ -2230,7 +2286,7 @@
       <c r="BK1" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="BL1" s="68" t="s">
+      <c r="BL1" s="65" t="s">
         <v>60</v>
       </c>
     </row>
@@ -2244,7 +2300,7 @@
       <c r="E2" s="58" t="s">
         <v>107</v>
       </c>
-      <c r="F2" s="79" t="s">
+      <c r="F2" s="76" t="s">
         <v>4</v>
       </c>
       <c r="G2" s="58"/>
@@ -2279,37 +2335,37 @@
         <v>74</v>
       </c>
       <c r="T2" s="22"/>
-      <c r="BL2" s="69"/>
+      <c r="BL2" s="66"/>
     </row>
     <row r="3" spans="1:64" ht="16" customHeight="1" thickTop="1">
       <c r="A3" s="2">
         <v>19</v>
       </c>
-      <c r="B3" s="63" t="s">
+      <c r="B3" s="100" t="s">
         <v>72</v>
       </c>
       <c r="C3" s="11">
         <v>1</v>
       </c>
-      <c r="D3" s="80"/>
-      <c r="E3" s="80"/>
-      <c r="F3" s="73">
+      <c r="D3" s="77"/>
+      <c r="E3" s="77"/>
+      <c r="F3" s="70">
         <v>5.5</v>
       </c>
-      <c r="G3" s="76">
+      <c r="G3" s="73">
         <v>9.6999999999999993</v>
       </c>
-      <c r="H3" s="99">
+      <c r="H3" s="96">
         <v>16700</v>
       </c>
-      <c r="I3" s="81"/>
-      <c r="J3" s="81"/>
-      <c r="K3" s="82"/>
-      <c r="L3" s="83"/>
-      <c r="M3" s="83"/>
-      <c r="N3" s="83"/>
-      <c r="O3" s="84"/>
-      <c r="P3" s="84" t="s">
+      <c r="I3" s="78"/>
+      <c r="J3" s="78"/>
+      <c r="K3" s="79"/>
+      <c r="L3" s="80"/>
+      <c r="M3" s="80"/>
+      <c r="N3" s="80"/>
+      <c r="O3" s="81"/>
+      <c r="P3" s="81" t="s">
         <v>120</v>
       </c>
       <c r="R3" s="14" t="s">
@@ -2339,10 +2395,18 @@
       <c r="AA3" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="AB3" s="25"/>
-      <c r="AC3" s="25"/>
-      <c r="AD3" s="25"/>
-      <c r="AE3" s="25"/>
+      <c r="AB3" s="25">
+        <v>67169028</v>
+      </c>
+      <c r="AC3" s="25">
+        <v>67169028</v>
+      </c>
+      <c r="AD3" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="AE3" s="25" t="s">
+        <v>135</v>
+      </c>
       <c r="AF3" s="26" t="s">
         <v>33</v>
       </c>
@@ -2418,7 +2482,7 @@
       <c r="BD3" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="BE3" s="66">
+      <c r="BE3" s="63">
         <v>41001</v>
       </c>
       <c r="BF3" s="22">
@@ -2436,7 +2500,7 @@
       <c r="BK3" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="BL3" s="70" t="s">
+      <c r="BL3" s="67" t="s">
         <v>62</v>
       </c>
     </row>
@@ -2444,29 +2508,29 @@
       <c r="A4" s="3">
         <v>21</v>
       </c>
-      <c r="B4" s="64"/>
+      <c r="B4" s="101"/>
       <c r="C4" s="12">
         <v>4</v>
       </c>
-      <c r="D4" s="85"/>
-      <c r="E4" s="85"/>
-      <c r="F4" s="74">
+      <c r="D4" s="82"/>
+      <c r="E4" s="82"/>
+      <c r="F4" s="71">
         <v>11.4</v>
       </c>
-      <c r="G4" s="77">
+      <c r="G4" s="74">
         <v>10.15</v>
       </c>
-      <c r="H4" s="100">
+      <c r="H4" s="97">
         <v>16000</v>
       </c>
-      <c r="I4" s="86"/>
-      <c r="J4" s="86"/>
-      <c r="K4" s="87"/>
-      <c r="L4" s="88"/>
-      <c r="M4" s="88"/>
-      <c r="N4" s="88"/>
-      <c r="O4" s="89"/>
-      <c r="P4" s="89" t="s">
+      <c r="I4" s="83"/>
+      <c r="J4" s="83"/>
+      <c r="K4" s="84"/>
+      <c r="L4" s="85"/>
+      <c r="M4" s="85"/>
+      <c r="N4" s="85"/>
+      <c r="O4" s="86"/>
+      <c r="P4" s="86" t="s">
         <v>120</v>
       </c>
       <c r="R4" s="14" t="s">
@@ -2496,10 +2560,18 @@
       <c r="AA4" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="AB4" s="25"/>
-      <c r="AC4" s="25"/>
-      <c r="AD4" s="25"/>
-      <c r="AE4" s="25"/>
+      <c r="AB4" s="25">
+        <v>37585237</v>
+      </c>
+      <c r="AC4" s="25">
+        <v>37585237</v>
+      </c>
+      <c r="AD4" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="AE4" s="25" t="s">
+        <v>136</v>
+      </c>
       <c r="AF4" s="26" t="s">
         <v>33</v>
       </c>
@@ -2575,7 +2647,7 @@
       <c r="BD4" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="BE4" s="66">
+      <c r="BE4" s="63">
         <v>41043</v>
       </c>
       <c r="BF4" s="22">
@@ -2593,7 +2665,7 @@
       <c r="BK4" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="BL4" s="70" t="s">
+      <c r="BL4" s="67" t="s">
         <v>62</v>
       </c>
     </row>
@@ -2601,29 +2673,29 @@
       <c r="A5" s="3">
         <v>23</v>
       </c>
-      <c r="B5" s="64"/>
+      <c r="B5" s="101"/>
       <c r="C5" s="12">
         <v>10</v>
       </c>
-      <c r="D5" s="85"/>
-      <c r="E5" s="85"/>
-      <c r="F5" s="74">
+      <c r="D5" s="82"/>
+      <c r="E5" s="82"/>
+      <c r="F5" s="71">
         <v>25.6</v>
       </c>
-      <c r="G5" s="77">
+      <c r="G5" s="74">
         <v>10.199999999999999</v>
       </c>
-      <c r="H5" s="100">
+      <c r="H5" s="97">
         <v>7900</v>
       </c>
-      <c r="I5" s="86"/>
-      <c r="J5" s="86"/>
-      <c r="K5" s="87"/>
-      <c r="L5" s="88"/>
-      <c r="M5" s="88"/>
-      <c r="N5" s="88"/>
-      <c r="O5" s="89"/>
-      <c r="P5" s="89" t="s">
+      <c r="I5" s="83"/>
+      <c r="J5" s="83"/>
+      <c r="K5" s="84"/>
+      <c r="L5" s="85"/>
+      <c r="M5" s="85"/>
+      <c r="N5" s="85"/>
+      <c r="O5" s="86"/>
+      <c r="P5" s="86" t="s">
         <v>120</v>
       </c>
       <c r="R5" s="14" t="s">
@@ -2653,10 +2725,18 @@
       <c r="AA5" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="AB5" s="25"/>
-      <c r="AC5" s="25"/>
-      <c r="AD5" s="25"/>
-      <c r="AE5" s="25"/>
+      <c r="AB5" s="25">
+        <v>73593472</v>
+      </c>
+      <c r="AC5" s="25">
+        <v>73593472</v>
+      </c>
+      <c r="AD5" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="AE5" s="25" t="s">
+        <v>137</v>
+      </c>
       <c r="AF5" s="26" t="s">
         <v>33</v>
       </c>
@@ -2732,7 +2812,7 @@
       <c r="BD5" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="BE5" s="66">
+      <c r="BE5" s="63">
         <v>41127</v>
       </c>
       <c r="BF5" s="22">
@@ -2750,7 +2830,7 @@
       <c r="BK5" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="BL5" s="70" t="s">
+      <c r="BL5" s="67" t="s">
         <v>62</v>
       </c>
     </row>
@@ -2758,41 +2838,41 @@
       <c r="A6" s="3">
         <v>25</v>
       </c>
-      <c r="B6" s="64"/>
+      <c r="B6" s="101"/>
       <c r="C6" s="12">
         <v>12</v>
       </c>
-      <c r="D6" s="85"/>
-      <c r="E6" s="85"/>
-      <c r="F6" s="90">
+      <c r="D6" s="82"/>
+      <c r="E6" s="82"/>
+      <c r="F6" s="87">
         <v>18.100000000000001</v>
       </c>
-      <c r="G6" s="85">
+      <c r="G6" s="82">
         <v>10.26</v>
       </c>
-      <c r="H6" s="101">
+      <c r="H6" s="98">
         <v>19300</v>
       </c>
-      <c r="I6" s="86">
+      <c r="I6" s="83">
         <v>10569</v>
       </c>
-      <c r="J6" s="86">
+      <c r="J6" s="83">
         <v>3039</v>
       </c>
-      <c r="K6" s="87">
+      <c r="K6" s="84">
         <v>4525</v>
       </c>
-      <c r="L6" s="88">
+      <c r="L6" s="85">
         <v>1075</v>
       </c>
-      <c r="M6" s="88">
+      <c r="M6" s="85">
         <v>962</v>
       </c>
-      <c r="N6" s="88">
+      <c r="N6" s="85">
         <v>160.69999999999999</v>
       </c>
-      <c r="O6" s="89"/>
-      <c r="P6" s="89" t="s">
+      <c r="O6" s="86"/>
+      <c r="P6" s="86" t="s">
         <v>120</v>
       </c>
       <c r="R6" s="14" t="s">
@@ -2822,10 +2902,18 @@
       <c r="AA6" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="AB6" s="25"/>
-      <c r="AC6" s="25"/>
-      <c r="AD6" s="25"/>
-      <c r="AE6" s="25"/>
+      <c r="AB6" s="25">
+        <v>45978734</v>
+      </c>
+      <c r="AC6" s="25">
+        <v>45978734</v>
+      </c>
+      <c r="AD6" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="AE6" s="25" t="s">
+        <v>138</v>
+      </c>
       <c r="AF6" s="26" t="s">
         <v>33</v>
       </c>
@@ -2901,7 +2989,7 @@
       <c r="BD6" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="BE6" s="66">
+      <c r="BE6" s="63">
         <v>41162</v>
       </c>
       <c r="BF6" s="22">
@@ -2919,7 +3007,7 @@
       <c r="BK6" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="BL6" s="70" t="s">
+      <c r="BL6" s="67" t="s">
         <v>62</v>
       </c>
     </row>
@@ -2927,49 +3015,49 @@
       <c r="A7" s="2">
         <v>35</v>
       </c>
-      <c r="B7" s="63" t="s">
+      <c r="B7" s="100" t="s">
         <v>73</v>
       </c>
       <c r="C7" s="11">
         <v>1</v>
       </c>
-      <c r="D7" s="91">
+      <c r="D7" s="88">
         <v>1125.0000000000011</v>
       </c>
-      <c r="E7" s="91">
+      <c r="E7" s="88">
         <v>202.20349999999999</v>
       </c>
-      <c r="F7" s="90">
+      <c r="F7" s="87">
         <v>3.2</v>
       </c>
-      <c r="G7" s="85">
+      <c r="G7" s="82">
         <v>9.8000000000000007</v>
       </c>
-      <c r="H7" s="101">
+      <c r="H7" s="98">
         <v>13200</v>
       </c>
-      <c r="I7" s="86">
+      <c r="I7" s="83">
         <v>3321</v>
       </c>
-      <c r="J7" s="86">
+      <c r="J7" s="83">
         <v>2294</v>
       </c>
-      <c r="K7" s="87">
+      <c r="K7" s="84">
         <v>3320</v>
       </c>
-      <c r="L7" s="88">
+      <c r="L7" s="85">
         <v>558</v>
       </c>
-      <c r="M7" s="88">
+      <c r="M7" s="85">
         <v>1430</v>
       </c>
-      <c r="N7" s="88">
+      <c r="N7" s="85">
         <v>182.8</v>
       </c>
-      <c r="O7" s="84">
+      <c r="O7" s="81">
         <v>329062500</v>
       </c>
-      <c r="P7" s="84" t="s">
+      <c r="P7" s="81" t="s">
         <v>119</v>
       </c>
       <c r="Q7" s="34"/>
@@ -3000,10 +3088,18 @@
       <c r="AA7" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="AB7" s="36"/>
-      <c r="AC7" s="36"/>
-      <c r="AD7" s="36"/>
-      <c r="AE7" s="36"/>
+      <c r="AB7" s="36">
+        <v>124471218</v>
+      </c>
+      <c r="AC7" s="36">
+        <v>124471218</v>
+      </c>
+      <c r="AD7" s="36" t="s">
+        <v>131</v>
+      </c>
+      <c r="AE7" s="36" t="s">
+        <v>139</v>
+      </c>
       <c r="AF7" s="37" t="s">
         <v>33</v>
       </c>
@@ -3079,7 +3175,7 @@
       <c r="BD7" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="BE7" s="66">
+      <c r="BE7" s="63">
         <v>41001</v>
       </c>
       <c r="BF7" s="35">
@@ -3098,7 +3194,7 @@
       <c r="BK7" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="BL7" s="70" t="s">
+      <c r="BL7" s="67" t="s">
         <v>62</v>
       </c>
     </row>
@@ -3106,47 +3202,47 @@
       <c r="A8" s="3">
         <v>37</v>
       </c>
-      <c r="B8" s="64"/>
+      <c r="B8" s="101"/>
       <c r="C8" s="13">
         <v>2</v>
       </c>
-      <c r="D8" s="85">
+      <c r="D8" s="82">
         <v>285.71428571428595</v>
       </c>
-      <c r="E8" s="85">
+      <c r="E8" s="82">
         <v>226.0694</v>
       </c>
-      <c r="F8" s="90">
+      <c r="F8" s="87">
         <v>9.1999999999999993</v>
       </c>
-      <c r="G8" s="85">
+      <c r="G8" s="82">
         <v>10.1</v>
       </c>
-      <c r="H8" s="101">
+      <c r="H8" s="98">
         <v>14300</v>
       </c>
-      <c r="I8" s="86">
+      <c r="I8" s="83">
         <v>1059</v>
       </c>
-      <c r="J8" s="86">
+      <c r="J8" s="83">
         <v>1137</v>
       </c>
-      <c r="K8" s="87">
+      <c r="K8" s="84">
         <v>3448</v>
       </c>
-      <c r="L8" s="88">
+      <c r="L8" s="85">
         <v>675</v>
       </c>
-      <c r="M8" s="88">
+      <c r="M8" s="85">
         <v>850</v>
       </c>
-      <c r="N8" s="88">
+      <c r="N8" s="85">
         <v>45.4</v>
       </c>
-      <c r="O8" s="89">
+      <c r="O8" s="86">
         <v>281812500</v>
       </c>
-      <c r="P8" s="89" t="s">
+      <c r="P8" s="86" t="s">
         <v>119</v>
       </c>
       <c r="Q8" s="34"/>
@@ -3177,10 +3273,18 @@
       <c r="AA8" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="AB8" s="36"/>
-      <c r="AC8" s="36"/>
-      <c r="AD8" s="36"/>
-      <c r="AE8" s="36"/>
+      <c r="AB8" s="36">
+        <v>37770014</v>
+      </c>
+      <c r="AC8" s="36">
+        <v>37770014</v>
+      </c>
+      <c r="AD8" s="36" t="s">
+        <v>132</v>
+      </c>
+      <c r="AE8" s="36" t="s">
+        <v>140</v>
+      </c>
       <c r="AF8" s="37" t="s">
         <v>33</v>
       </c>
@@ -3256,7 +3360,7 @@
       <c r="BD8" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="BE8" s="66">
+      <c r="BE8" s="63">
         <v>41015</v>
       </c>
       <c r="BF8" s="35">
@@ -3275,7 +3379,7 @@
       <c r="BK8" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="BL8" s="70" t="s">
+      <c r="BL8" s="67" t="s">
         <v>62</v>
       </c>
     </row>
@@ -3283,47 +3387,47 @@
       <c r="A9" s="3">
         <v>39</v>
       </c>
-      <c r="B9" s="64"/>
+      <c r="B9" s="101"/>
       <c r="C9" s="13">
         <v>12</v>
       </c>
-      <c r="D9" s="85">
+      <c r="D9" s="82">
         <v>900.0000000000008</v>
       </c>
-      <c r="E9" s="85">
+      <c r="E9" s="82">
         <v>414.01119999999997</v>
       </c>
-      <c r="F9" s="90">
+      <c r="F9" s="87">
         <v>15.1</v>
       </c>
-      <c r="G9" s="85">
+      <c r="G9" s="82">
         <v>10.16</v>
       </c>
-      <c r="H9" s="101">
+      <c r="H9" s="98">
         <v>35700</v>
       </c>
-      <c r="I9" s="86">
+      <c r="I9" s="83">
         <v>5323</v>
       </c>
-      <c r="J9" s="86">
+      <c r="J9" s="83">
         <v>9420</v>
       </c>
-      <c r="K9" s="87">
+      <c r="K9" s="84">
         <v>6040</v>
       </c>
-      <c r="L9" s="88">
+      <c r="L9" s="85">
         <v>1480</v>
       </c>
-      <c r="M9" s="88">
+      <c r="M9" s="85">
         <v>2400</v>
       </c>
-      <c r="N9" s="88">
+      <c r="N9" s="85">
         <v>723</v>
       </c>
-      <c r="O9" s="89">
+      <c r="O9" s="86">
         <v>81000000</v>
       </c>
-      <c r="P9" s="89" t="s">
+      <c r="P9" s="86" t="s">
         <v>119</v>
       </c>
       <c r="Q9" s="34"/>
@@ -3354,10 +3458,18 @@
       <c r="AA9" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="AB9" s="36"/>
-      <c r="AC9" s="36"/>
-      <c r="AD9" s="36"/>
-      <c r="AE9" s="36"/>
+      <c r="AB9" s="36">
+        <v>58650577</v>
+      </c>
+      <c r="AC9" s="36">
+        <v>58650577</v>
+      </c>
+      <c r="AD9" s="36" t="s">
+        <v>133</v>
+      </c>
+      <c r="AE9" s="36" t="s">
+        <v>141</v>
+      </c>
       <c r="AF9" s="37" t="s">
         <v>33</v>
       </c>
@@ -3433,7 +3545,7 @@
       <c r="BD9" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="BE9" s="66">
+      <c r="BE9" s="63">
         <v>41162</v>
       </c>
       <c r="BF9" s="35">
@@ -3452,7 +3564,7 @@
       <c r="BK9" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="BL9" s="70" t="s">
+      <c r="BL9" s="67" t="s">
         <v>62</v>
       </c>
     </row>
@@ -3460,37 +3572,37 @@
       <c r="A10" s="3">
         <v>41</v>
       </c>
-      <c r="B10" s="65"/>
+      <c r="B10" s="102"/>
       <c r="C10" s="43">
         <v>24</v>
       </c>
-      <c r="D10" s="92">
+      <c r="D10" s="89">
         <v>143.99999999999969</v>
       </c>
-      <c r="E10" s="92">
+      <c r="E10" s="89">
         <v>22.957250000000002</v>
       </c>
-      <c r="F10" s="93">
+      <c r="F10" s="90">
         <v>1.4</v>
       </c>
-      <c r="G10" s="94">
+      <c r="G10" s="91">
         <v>8.9</v>
       </c>
-      <c r="H10" s="102">
+      <c r="H10" s="99">
         <v>1900</v>
       </c>
-      <c r="I10" s="92"/>
-      <c r="J10" s="92"/>
-      <c r="K10" s="95"/>
-      <c r="L10" s="96"/>
-      <c r="M10" s="97">
+      <c r="I10" s="89"/>
+      <c r="J10" s="89"/>
+      <c r="K10" s="92"/>
+      <c r="L10" s="93"/>
+      <c r="M10" s="94">
         <v>240</v>
       </c>
-      <c r="N10" s="97">
+      <c r="N10" s="94">
         <v>31.4</v>
       </c>
-      <c r="O10" s="98"/>
-      <c r="P10" s="98" t="s">
+      <c r="O10" s="95"/>
+      <c r="P10" s="95" t="s">
         <v>119</v>
       </c>
       <c r="Q10" s="44"/>
@@ -3524,10 +3636,18 @@
       <c r="AA10" s="48" t="s">
         <v>92</v>
       </c>
-      <c r="AB10" s="48"/>
-      <c r="AC10" s="48"/>
-      <c r="AD10" s="48"/>
-      <c r="AE10" s="48"/>
+      <c r="AB10" s="48">
+        <v>51786260</v>
+      </c>
+      <c r="AC10" s="48">
+        <v>51786260</v>
+      </c>
+      <c r="AD10" s="48" t="s">
+        <v>134</v>
+      </c>
+      <c r="AE10" s="48" t="s">
+        <v>142</v>
+      </c>
       <c r="AF10" s="49" t="s">
         <v>33</v>
       </c>
@@ -3603,7 +3723,7 @@
       <c r="BD10" s="56" t="s">
         <v>65</v>
       </c>
-      <c r="BE10" s="67">
+      <c r="BE10" s="64">
         <v>41309</v>
       </c>
       <c r="BF10" s="47">
@@ -3622,7 +3742,7 @@
       <c r="BK10" s="56" t="s">
         <v>61</v>
       </c>
-      <c r="BL10" s="71" t="s">
+      <c r="BL10" s="68" t="s">
         <v>62</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update metadata design description
</commit_message>
<xml_diff>
--- a/scripts/projects/soda_rerun/meta_data.xlsx
+++ b/scripts/projects/soda_rerun/meta_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="28720" windowHeight="9200"/>
+    <workbookView xWindow="760" yWindow="0" windowWidth="28700" windowHeight="16980"/>
   </bookViews>
   <sheets>
     <sheet name="SUMMARY.csv" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="144">
   <si>
     <t>Sample</t>
   </si>
@@ -48,9 +48,6 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Shotgun</t>
-  </si>
-  <si>
     <t>Run name</t>
   </si>
   <si>
@@ -448,6 +445,12 @@
   </si>
   <si>
     <t>1be86e35b31b69037545bbf7417e8811</t>
+  </si>
+  <si>
+    <t>16S</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -1141,7 +1144,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="57">
+  <cellStyleXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1216,6 +1219,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1604,7 +1613,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="57">
+  <cellStyles count="59">
     <cellStyle name="Excel Built-in Normal" xfId="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -1646,6 +1655,7 @@
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
@@ -1661,6 +1671,7 @@
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="1">
@@ -2073,10 +2084,10 @@
   <dimension ref="A1:BL11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="V2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AB15" sqref="AB15"/>
+      <selection pane="bottomRight" activeCell="S23" sqref="S23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2124,10 +2135,10 @@
         <v>5</v>
       </c>
       <c r="D1" s="57" t="s">
+        <v>104</v>
+      </c>
+      <c r="E1" s="57" t="s">
         <v>105</v>
-      </c>
-      <c r="E1" s="57" t="s">
-        <v>106</v>
       </c>
       <c r="F1" s="75" t="s">
         <v>2</v>
@@ -2136,169 +2147,169 @@
         <v>1</v>
       </c>
       <c r="H1" s="57" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I1" s="57" t="s">
+        <v>107</v>
+      </c>
+      <c r="J1" s="57" t="s">
         <v>108</v>
       </c>
-      <c r="J1" s="57" t="s">
+      <c r="K1" s="61" t="s">
         <v>109</v>
       </c>
-      <c r="K1" s="61" t="s">
+      <c r="L1" s="59" t="s">
         <v>110</v>
       </c>
-      <c r="L1" s="59" t="s">
+      <c r="M1" s="69" t="s">
         <v>111</v>
       </c>
-      <c r="M1" s="69" t="s">
+      <c r="N1" s="69" t="s">
         <v>112</v>
-      </c>
-      <c r="N1" s="69" t="s">
-        <v>113</v>
       </c>
       <c r="O1" s="9" t="s">
         <v>3</v>
       </c>
       <c r="P1" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="S1" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="T1" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="U1" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="T1" s="19" t="s">
+      <c r="V1" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="W1" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="X1" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="Y1" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="Z1" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="U1" s="19" t="s">
+      <c r="AA1" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB1" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="AC1" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD1" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="AE1" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="AF1" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="AG1" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="AH1" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="AI1" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="AJ1" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="AK1" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="AL1" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="AM1" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="AN1" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="AO1" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="AP1" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="AQ1" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="V1" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="W1" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="X1" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="Y1" s="19" t="s">
-        <v>125</v>
-      </c>
-      <c r="Z1" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="AA1" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB1" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="AC1" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="AD1" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="AE1" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="AF1" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="AG1" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="AH1" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="AI1" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="AJ1" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="AK1" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="AL1" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="AM1" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="AN1" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="AO1" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="AP1" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="AQ1" s="19" t="s">
-        <v>11</v>
-      </c>
       <c r="AR1" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AS1" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="AS1" s="19" t="s">
+      <c r="AT1" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="AT1" s="19" t="s">
+      <c r="AU1" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="AU1" s="19" t="s">
+      <c r="AV1" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="AV1" s="19" t="s">
+      <c r="AW1" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="AW1" s="19" t="s">
+      <c r="AX1" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="AX1" s="19" t="s">
+      <c r="AY1" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="AY1" s="19" t="s">
+      <c r="AZ1" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="AZ1" s="19" t="s">
-        <v>45</v>
-      </c>
       <c r="BA1" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="BB1" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="BC1" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="BD1" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="BB1" s="30" t="s">
+      <c r="BE1" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="BF1" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="BG1" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="BH1" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="BC1" s="30" t="s">
-        <v>54</v>
-      </c>
-      <c r="BD1" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="BE1" s="33" t="s">
-        <v>67</v>
-      </c>
-      <c r="BF1" s="33" t="s">
-        <v>68</v>
-      </c>
-      <c r="BG1" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="BH1" s="31" t="s">
+      <c r="BI1" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="BI1" s="31" t="s">
+      <c r="BJ1" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="BJ1" s="31" t="s">
+      <c r="BK1" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="BK1" s="32" t="s">
+      <c r="BL1" s="65" t="s">
         <v>59</v>
-      </c>
-      <c r="BL1" s="65" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:64" ht="16" customHeight="1" thickBot="1">
@@ -2306,44 +2317,44 @@
       <c r="B2" s="7"/>
       <c r="C2" s="8"/>
       <c r="D2" s="58" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E2" s="58" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F2" s="76" t="s">
         <v>4</v>
       </c>
       <c r="G2" s="58"/>
       <c r="H2" s="58" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I2" s="58" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J2" s="58" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K2" s="62" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="L2" s="60" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M2" s="58" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="N2" s="58" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="O2" s="10" t="s">
         <v>7</v>
       </c>
       <c r="P2" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="S2" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="T2" s="22"/>
       <c r="BL2" s="66"/>
@@ -2353,7 +2364,7 @@
         <v>19</v>
       </c>
       <c r="B3" s="103" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C3" s="11">
         <v>1</v>
@@ -2377,34 +2388,34 @@
       <c r="N3" s="80"/>
       <c r="O3" s="81"/>
       <c r="P3" s="81" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="R3" s="14" t="s">
         <v>8</v>
       </c>
       <c r="S3" s="17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="T3" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="U3" t="s">
+        <v>81</v>
+      </c>
+      <c r="V3" t="s">
         <v>82</v>
       </c>
-      <c r="V3" t="s">
-        <v>83</v>
-      </c>
       <c r="W3" t="s">
+        <v>89</v>
+      </c>
+      <c r="X3" t="s">
+        <v>116</v>
+      </c>
+      <c r="Z3" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="X3" t="s">
-        <v>117</v>
-      </c>
-      <c r="Z3" s="25" t="s">
+      <c r="AA3" s="25" t="s">
         <v>91</v>
-      </c>
-      <c r="AA3" s="25" t="s">
-        <v>92</v>
       </c>
       <c r="AB3" s="100">
         <v>67169028</v>
@@ -2413,67 +2424,67 @@
         <v>67169028</v>
       </c>
       <c r="AD3" s="25" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AE3" s="25" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AF3" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="AG3" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="AH3" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI3" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="AG3" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH3" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="AI3" s="26" t="s">
+      <c r="AJ3" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="AJ3" s="27" t="s">
+      <c r="AK3" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="AK3" s="29" t="s">
-        <v>36</v>
-      </c>
       <c r="AL3" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="AM3" s="21" t="s">
         <v>93</v>
-      </c>
-      <c r="AM3" s="21" t="s">
-        <v>94</v>
       </c>
       <c r="AN3" s="21">
         <v>7</v>
       </c>
       <c r="AO3" s="24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="AP3" s="22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AQ3" s="24">
         <v>1</v>
       </c>
       <c r="AR3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AS3" t="s">
         <v>46</v>
       </c>
-      <c r="AS3" t="s">
+      <c r="AT3" t="s">
         <v>47</v>
       </c>
-      <c r="AT3" t="s">
+      <c r="AU3" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="AU3" s="23" t="s">
+      <c r="AV3" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="AV3" s="23" t="s">
+      <c r="AW3" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="AW3" s="23" t="s">
-        <v>51</v>
-      </c>
       <c r="AX3" s="23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AY3" s="23">
         <v>125</v>
@@ -2482,16 +2493,16 @@
         <v>125</v>
       </c>
       <c r="BA3" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="BB3" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="BB3" s="23" t="s">
+      <c r="BC3" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="BD3" s="23" t="s">
         <v>64</v>
-      </c>
-      <c r="BC3" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="BD3" s="23" t="s">
-        <v>65</v>
       </c>
       <c r="BE3" s="63">
         <v>41001</v>
@@ -2503,16 +2514,19 @@
         <v>16.780556000000001</v>
       </c>
       <c r="BH3" t="s">
+        <v>102</v>
+      </c>
+      <c r="BI3" t="s">
         <v>103</v>
       </c>
-      <c r="BI3" t="s">
-        <v>104</v>
+      <c r="BJ3" t="s">
+        <v>143</v>
       </c>
       <c r="BK3" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="BL3" s="67" t="s">
         <v>61</v>
-      </c>
-      <c r="BL3" s="67" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:64" ht="15" customHeight="1">
@@ -2542,34 +2556,34 @@
       <c r="N4" s="85"/>
       <c r="O4" s="86"/>
       <c r="P4" s="86" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="R4" s="14" t="s">
         <v>8</v>
       </c>
       <c r="S4" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="T4" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="U4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="V4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="W4" t="s">
+        <v>89</v>
+      </c>
+      <c r="X4" t="s">
+        <v>116</v>
+      </c>
+      <c r="Z4" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="X4" t="s">
-        <v>117</v>
-      </c>
-      <c r="Z4" s="25" t="s">
+      <c r="AA4" s="25" t="s">
         <v>91</v>
-      </c>
-      <c r="AA4" s="25" t="s">
-        <v>92</v>
       </c>
       <c r="AB4" s="100">
         <v>37585237</v>
@@ -2578,67 +2592,67 @@
         <v>37585237</v>
       </c>
       <c r="AD4" s="25" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AE4" s="25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AF4" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="AG4" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="AH4" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI4" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="AG4" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH4" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="AI4" s="26" t="s">
+      <c r="AJ4" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="AJ4" s="27" t="s">
+      <c r="AK4" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="AK4" s="29" t="s">
-        <v>36</v>
-      </c>
       <c r="AL4" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="AM4" s="21" t="s">
         <v>93</v>
-      </c>
-      <c r="AM4" s="21" t="s">
-        <v>94</v>
       </c>
       <c r="AN4" s="21">
         <v>7</v>
       </c>
       <c r="AO4" s="24" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AP4" s="22" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AQ4" s="24">
         <v>2</v>
       </c>
       <c r="AR4" t="s">
+        <v>45</v>
+      </c>
+      <c r="AS4" t="s">
         <v>46</v>
       </c>
-      <c r="AS4" t="s">
+      <c r="AT4" t="s">
         <v>47</v>
       </c>
-      <c r="AT4" t="s">
+      <c r="AU4" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="AU4" s="23" t="s">
+      <c r="AV4" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="AV4" s="23" t="s">
+      <c r="AW4" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="AW4" s="23" t="s">
-        <v>51</v>
-      </c>
       <c r="AX4" s="23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AY4" s="23">
         <v>125</v>
@@ -2647,16 +2661,16 @@
         <v>125</v>
       </c>
       <c r="BA4" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="BB4" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="BB4" s="23" t="s">
+      <c r="BC4" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="BD4" s="23" t="s">
         <v>64</v>
-      </c>
-      <c r="BC4" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="BD4" s="23" t="s">
-        <v>65</v>
       </c>
       <c r="BE4" s="63">
         <v>41043</v>
@@ -2668,16 +2682,19 @@
         <v>16.780556000000001</v>
       </c>
       <c r="BH4" t="s">
+        <v>102</v>
+      </c>
+      <c r="BI4" t="s">
         <v>103</v>
       </c>
-      <c r="BI4" t="s">
-        <v>104</v>
+      <c r="BJ4" t="s">
+        <v>143</v>
       </c>
       <c r="BK4" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="BL4" s="67" t="s">
         <v>61</v>
-      </c>
-      <c r="BL4" s="67" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:64" ht="15" customHeight="1">
@@ -2707,34 +2724,34 @@
       <c r="N5" s="85"/>
       <c r="O5" s="86"/>
       <c r="P5" s="86" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="R5" s="14" t="s">
         <v>8</v>
       </c>
       <c r="S5" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="T5" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="U5" t="s">
         <v>81</v>
       </c>
-      <c r="T5" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="U5" t="s">
-        <v>82</v>
-      </c>
       <c r="V5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="W5" t="s">
+        <v>89</v>
+      </c>
+      <c r="X5" t="s">
+        <v>116</v>
+      </c>
+      <c r="Z5" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="X5" t="s">
-        <v>117</v>
-      </c>
-      <c r="Z5" s="25" t="s">
+      <c r="AA5" s="25" t="s">
         <v>91</v>
-      </c>
-      <c r="AA5" s="25" t="s">
-        <v>92</v>
       </c>
       <c r="AB5" s="100">
         <v>73593472</v>
@@ -2743,67 +2760,67 @@
         <v>73593472</v>
       </c>
       <c r="AD5" s="25" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AE5" s="25" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="AF5" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="AG5" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="AH5" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI5" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="AG5" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH5" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="AI5" s="26" t="s">
+      <c r="AJ5" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="AJ5" s="27" t="s">
+      <c r="AK5" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="AK5" s="29" t="s">
-        <v>36</v>
-      </c>
       <c r="AL5" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="AM5" s="21" t="s">
         <v>93</v>
-      </c>
-      <c r="AM5" s="21" t="s">
-        <v>94</v>
       </c>
       <c r="AN5" s="21">
         <v>7</v>
       </c>
       <c r="AO5" s="24" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AP5" s="22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AQ5" s="24">
         <v>3</v>
       </c>
       <c r="AR5" t="s">
+        <v>45</v>
+      </c>
+      <c r="AS5" t="s">
         <v>46</v>
       </c>
-      <c r="AS5" t="s">
+      <c r="AT5" t="s">
         <v>47</v>
       </c>
-      <c r="AT5" t="s">
+      <c r="AU5" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="AU5" s="23" t="s">
+      <c r="AV5" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="AV5" s="23" t="s">
+      <c r="AW5" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="AW5" s="23" t="s">
-        <v>51</v>
-      </c>
       <c r="AX5" s="23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AY5" s="23">
         <v>125</v>
@@ -2812,16 +2829,16 @@
         <v>125</v>
       </c>
       <c r="BA5" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="BB5" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="BB5" s="23" t="s">
+      <c r="BC5" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="BD5" s="23" t="s">
         <v>64</v>
-      </c>
-      <c r="BC5" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="BD5" s="23" t="s">
-        <v>65</v>
       </c>
       <c r="BE5" s="63">
         <v>41127</v>
@@ -2833,16 +2850,19 @@
         <v>16.780556000000001</v>
       </c>
       <c r="BH5" t="s">
+        <v>102</v>
+      </c>
+      <c r="BI5" t="s">
         <v>103</v>
       </c>
-      <c r="BI5" t="s">
-        <v>104</v>
+      <c r="BJ5" t="s">
+        <v>143</v>
       </c>
       <c r="BK5" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="BL5" s="67" t="s">
         <v>61</v>
-      </c>
-      <c r="BL5" s="67" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:64" ht="15" customHeight="1" thickBot="1">
@@ -2884,34 +2904,34 @@
       </c>
       <c r="O6" s="86"/>
       <c r="P6" s="86" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="R6" s="14" t="s">
         <v>8</v>
       </c>
       <c r="S6" s="18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="T6" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="U6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="V6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="W6" t="s">
+        <v>89</v>
+      </c>
+      <c r="X6" t="s">
+        <v>116</v>
+      </c>
+      <c r="Z6" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="X6" t="s">
-        <v>117</v>
-      </c>
-      <c r="Z6" s="25" t="s">
+      <c r="AA6" s="25" t="s">
         <v>91</v>
-      </c>
-      <c r="AA6" s="25" t="s">
-        <v>92</v>
       </c>
       <c r="AB6" s="100">
         <v>45978734</v>
@@ -2920,67 +2940,67 @@
         <v>45978734</v>
       </c>
       <c r="AD6" s="25" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AE6" s="25" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AF6" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="AG6" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="AH6" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI6" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="AG6" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH6" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="AI6" s="26" t="s">
+      <c r="AJ6" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="AJ6" s="27" t="s">
+      <c r="AK6" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="AK6" s="29" t="s">
-        <v>36</v>
-      </c>
       <c r="AL6" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="AM6" s="21" t="s">
         <v>93</v>
-      </c>
-      <c r="AM6" s="21" t="s">
-        <v>94</v>
       </c>
       <c r="AN6" s="21">
         <v>7</v>
       </c>
       <c r="AO6" s="24" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AP6" s="22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AQ6" s="24">
         <v>4</v>
       </c>
       <c r="AR6" t="s">
+        <v>45</v>
+      </c>
+      <c r="AS6" t="s">
         <v>46</v>
       </c>
-      <c r="AS6" t="s">
+      <c r="AT6" t="s">
         <v>47</v>
       </c>
-      <c r="AT6" t="s">
+      <c r="AU6" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="AU6" s="23" t="s">
+      <c r="AV6" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="AV6" s="23" t="s">
+      <c r="AW6" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="AW6" s="23" t="s">
-        <v>51</v>
-      </c>
       <c r="AX6" s="23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AY6" s="23">
         <v>125</v>
@@ -2989,16 +3009,16 @@
         <v>125</v>
       </c>
       <c r="BA6" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="BB6" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="BB6" s="23" t="s">
+      <c r="BC6" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="BD6" s="23" t="s">
         <v>64</v>
-      </c>
-      <c r="BC6" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="BD6" s="23" t="s">
-        <v>65</v>
       </c>
       <c r="BE6" s="63">
         <v>41162</v>
@@ -3010,16 +3030,19 @@
         <v>16.780556000000001</v>
       </c>
       <c r="BH6" t="s">
+        <v>102</v>
+      </c>
+      <c r="BI6" t="s">
         <v>103</v>
       </c>
-      <c r="BI6" t="s">
-        <v>104</v>
+      <c r="BJ6" t="s">
+        <v>143</v>
       </c>
       <c r="BK6" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="BL6" s="67" t="s">
         <v>61</v>
-      </c>
-      <c r="BL6" s="67" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:64" ht="16" customHeight="1" thickTop="1">
@@ -3027,7 +3050,7 @@
         <v>35</v>
       </c>
       <c r="B7" s="103" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C7" s="11">
         <v>1</v>
@@ -3069,35 +3092,35 @@
         <v>329062500</v>
       </c>
       <c r="P7" s="81" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="Q7" s="34"/>
       <c r="R7" s="14" t="s">
         <v>8</v>
       </c>
       <c r="S7" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="T7" s="35" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="U7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="V7" s="34" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="W7" t="s">
+        <v>89</v>
+      </c>
+      <c r="X7" t="s">
+        <v>116</v>
+      </c>
+      <c r="Z7" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="X7" t="s">
-        <v>117</v>
-      </c>
-      <c r="Z7" s="25" t="s">
+      <c r="AA7" s="25" t="s">
         <v>91</v>
-      </c>
-      <c r="AA7" s="25" t="s">
-        <v>92</v>
       </c>
       <c r="AB7" s="101">
         <v>124471218</v>
@@ -3106,67 +3129,67 @@
         <v>124471218</v>
       </c>
       <c r="AD7" s="36" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AE7" s="36" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AF7" s="37" t="s">
+        <v>32</v>
+      </c>
+      <c r="AG7" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="AH7" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI7" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="AG7" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH7" s="39" t="s">
-        <v>32</v>
-      </c>
-      <c r="AI7" s="37" t="s">
+      <c r="AJ7" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="AJ7" s="38" t="s">
+      <c r="AK7" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="AK7" s="40" t="s">
-        <v>36</v>
-      </c>
       <c r="AL7" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="AM7" s="21" t="s">
         <v>93</v>
-      </c>
-      <c r="AM7" s="21" t="s">
-        <v>94</v>
       </c>
       <c r="AN7" s="21">
         <v>7</v>
       </c>
       <c r="AO7" s="41" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AP7" s="35" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AQ7" s="41">
         <v>5</v>
       </c>
       <c r="AR7" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="AS7" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="AS7" s="34" t="s">
+      <c r="AT7" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="AT7" s="34" t="s">
+      <c r="AU7" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="AU7" s="42" t="s">
+      <c r="AV7" s="42" t="s">
         <v>49</v>
       </c>
-      <c r="AV7" s="42" t="s">
+      <c r="AW7" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="AW7" s="42" t="s">
-        <v>51</v>
-      </c>
       <c r="AX7" s="23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AY7" s="42">
         <v>125</v>
@@ -3175,16 +3198,16 @@
         <v>125</v>
       </c>
       <c r="BA7" s="42" t="s">
+        <v>62</v>
+      </c>
+      <c r="BB7" s="42" t="s">
         <v>63</v>
       </c>
-      <c r="BB7" s="42" t="s">
+      <c r="BC7" s="42" t="s">
+        <v>65</v>
+      </c>
+      <c r="BD7" s="42" t="s">
         <v>64</v>
-      </c>
-      <c r="BC7" s="42" t="s">
-        <v>66</v>
-      </c>
-      <c r="BD7" s="42" t="s">
-        <v>65</v>
       </c>
       <c r="BE7" s="63">
         <v>41001</v>
@@ -3196,17 +3219,19 @@
         <v>16.780833000000001</v>
       </c>
       <c r="BH7" t="s">
+        <v>102</v>
+      </c>
+      <c r="BI7" t="s">
         <v>103</v>
       </c>
-      <c r="BI7" t="s">
-        <v>104</v>
-      </c>
-      <c r="BJ7" s="34"/>
+      <c r="BJ7" t="s">
+        <v>143</v>
+      </c>
       <c r="BK7" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="BL7" s="67" t="s">
         <v>61</v>
-      </c>
-      <c r="BL7" s="67" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:64" ht="15" customHeight="1">
@@ -3254,35 +3279,35 @@
         <v>281812500</v>
       </c>
       <c r="P8" s="86" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="Q8" s="34"/>
       <c r="R8" s="14" t="s">
         <v>8</v>
       </c>
       <c r="S8" s="18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="T8" s="35" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="U8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="V8" s="34" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="W8" t="s">
+        <v>89</v>
+      </c>
+      <c r="X8" t="s">
+        <v>116</v>
+      </c>
+      <c r="Z8" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="X8" t="s">
-        <v>117</v>
-      </c>
-      <c r="Z8" s="25" t="s">
+      <c r="AA8" s="25" t="s">
         <v>91</v>
-      </c>
-      <c r="AA8" s="25" t="s">
-        <v>92</v>
       </c>
       <c r="AB8" s="101">
         <v>37770014</v>
@@ -3291,67 +3316,67 @@
         <v>37770014</v>
       </c>
       <c r="AD8" s="36" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AE8" s="36" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AF8" s="37" t="s">
+        <v>32</v>
+      </c>
+      <c r="AG8" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="AH8" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI8" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="AG8" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH8" s="39" t="s">
-        <v>32</v>
-      </c>
-      <c r="AI8" s="37" t="s">
+      <c r="AJ8" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="AJ8" s="38" t="s">
+      <c r="AK8" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="AK8" s="40" t="s">
-        <v>36</v>
-      </c>
       <c r="AL8" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="AM8" s="21" t="s">
         <v>93</v>
-      </c>
-      <c r="AM8" s="21" t="s">
-        <v>94</v>
       </c>
       <c r="AN8" s="21">
         <v>7</v>
       </c>
       <c r="AO8" s="41" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AP8" s="35" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AQ8" s="41">
         <v>6</v>
       </c>
       <c r="AR8" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="AS8" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="AS8" s="34" t="s">
+      <c r="AT8" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="AT8" s="34" t="s">
+      <c r="AU8" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="AU8" s="42" t="s">
+      <c r="AV8" s="42" t="s">
         <v>49</v>
       </c>
-      <c r="AV8" s="42" t="s">
+      <c r="AW8" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="AW8" s="42" t="s">
-        <v>51</v>
-      </c>
       <c r="AX8" s="23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AY8" s="42">
         <v>125</v>
@@ -3360,16 +3385,16 @@
         <v>125</v>
       </c>
       <c r="BA8" s="42" t="s">
+        <v>62</v>
+      </c>
+      <c r="BB8" s="42" t="s">
         <v>63</v>
       </c>
-      <c r="BB8" s="42" t="s">
+      <c r="BC8" s="42" t="s">
+        <v>65</v>
+      </c>
+      <c r="BD8" s="42" t="s">
         <v>64</v>
-      </c>
-      <c r="BC8" s="42" t="s">
-        <v>66</v>
-      </c>
-      <c r="BD8" s="42" t="s">
-        <v>65</v>
       </c>
       <c r="BE8" s="63">
         <v>41015</v>
@@ -3381,17 +3406,19 @@
         <v>16.780833000000001</v>
       </c>
       <c r="BH8" t="s">
+        <v>102</v>
+      </c>
+      <c r="BI8" t="s">
         <v>103</v>
       </c>
-      <c r="BI8" t="s">
-        <v>104</v>
-      </c>
-      <c r="BJ8" s="34"/>
+      <c r="BJ8" t="s">
+        <v>143</v>
+      </c>
       <c r="BK8" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="BL8" s="67" t="s">
         <v>61</v>
-      </c>
-      <c r="BL8" s="67" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:64" ht="15" customHeight="1">
@@ -3439,35 +3466,35 @@
         <v>81000000</v>
       </c>
       <c r="P9" s="86" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="Q9" s="34"/>
       <c r="R9" s="14" t="s">
         <v>8</v>
       </c>
       <c r="S9" s="18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="T9" s="35" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="U9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="V9" s="34" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="W9" t="s">
+        <v>89</v>
+      </c>
+      <c r="X9" t="s">
+        <v>116</v>
+      </c>
+      <c r="Z9" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="X9" t="s">
-        <v>117</v>
-      </c>
-      <c r="Z9" s="25" t="s">
+      <c r="AA9" s="25" t="s">
         <v>91</v>
-      </c>
-      <c r="AA9" s="25" t="s">
-        <v>92</v>
       </c>
       <c r="AB9" s="101">
         <v>58650577</v>
@@ -3476,67 +3503,67 @@
         <v>58650577</v>
       </c>
       <c r="AD9" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AE9" s="36" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AF9" s="37" t="s">
+        <v>32</v>
+      </c>
+      <c r="AG9" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="AH9" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI9" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="AG9" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH9" s="39" t="s">
-        <v>32</v>
-      </c>
-      <c r="AI9" s="37" t="s">
+      <c r="AJ9" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="AJ9" s="38" t="s">
+      <c r="AK9" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="AK9" s="40" t="s">
-        <v>36</v>
-      </c>
       <c r="AL9" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="AM9" s="21" t="s">
         <v>93</v>
-      </c>
-      <c r="AM9" s="21" t="s">
-        <v>94</v>
       </c>
       <c r="AN9" s="21">
         <v>7</v>
       </c>
       <c r="AO9" s="41" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AP9" s="35" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AQ9" s="41">
         <v>7</v>
       </c>
       <c r="AR9" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="AS9" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="AS9" s="34" t="s">
+      <c r="AT9" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="AT9" s="34" t="s">
+      <c r="AU9" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="AU9" s="42" t="s">
+      <c r="AV9" s="42" t="s">
         <v>49</v>
       </c>
-      <c r="AV9" s="42" t="s">
+      <c r="AW9" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="AW9" s="42" t="s">
-        <v>51</v>
-      </c>
       <c r="AX9" s="23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AY9" s="42">
         <v>125</v>
@@ -3545,16 +3572,16 @@
         <v>125</v>
       </c>
       <c r="BA9" s="42" t="s">
+        <v>62</v>
+      </c>
+      <c r="BB9" s="42" t="s">
         <v>63</v>
       </c>
-      <c r="BB9" s="42" t="s">
+      <c r="BC9" s="42" t="s">
+        <v>65</v>
+      </c>
+      <c r="BD9" s="42" t="s">
         <v>64</v>
-      </c>
-      <c r="BC9" s="42" t="s">
-        <v>66</v>
-      </c>
-      <c r="BD9" s="42" t="s">
-        <v>65</v>
       </c>
       <c r="BE9" s="63">
         <v>41162</v>
@@ -3566,17 +3593,19 @@
         <v>16.780833000000001</v>
       </c>
       <c r="BH9" t="s">
+        <v>102</v>
+      </c>
+      <c r="BI9" t="s">
         <v>103</v>
       </c>
-      <c r="BI9" t="s">
-        <v>104</v>
-      </c>
-      <c r="BJ9" s="34"/>
+      <c r="BJ9" t="s">
+        <v>143</v>
+      </c>
       <c r="BK9" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="BL9" s="67" t="s">
         <v>61</v>
-      </c>
-      <c r="BL9" s="67" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:64" ht="15" customHeight="1" thickBot="1">
@@ -3614,38 +3643,38 @@
       </c>
       <c r="O10" s="95"/>
       <c r="P10" s="95" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="Q10" s="44"/>
       <c r="R10" s="45" t="s">
         <v>8</v>
       </c>
       <c r="S10" s="46" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="T10" s="47" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="U10" s="44" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="V10" s="44" t="s">
+        <v>88</v>
+      </c>
+      <c r="W10" s="44" t="s">
         <v>89</v>
       </c>
-      <c r="W10" s="44" t="s">
+      <c r="X10" s="44" t="s">
+        <v>116</v>
+      </c>
+      <c r="Y10" s="44" t="s">
+        <v>125</v>
+      </c>
+      <c r="Z10" s="48" t="s">
         <v>90</v>
       </c>
-      <c r="X10" s="44" t="s">
-        <v>117</v>
-      </c>
-      <c r="Y10" s="44" t="s">
-        <v>126</v>
-      </c>
-      <c r="Z10" s="48" t="s">
+      <c r="AA10" s="48" t="s">
         <v>91</v>
-      </c>
-      <c r="AA10" s="48" t="s">
-        <v>92</v>
       </c>
       <c r="AB10" s="102">
         <v>51786260</v>
@@ -3654,67 +3683,67 @@
         <v>51786260</v>
       </c>
       <c r="AD10" s="48" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AE10" s="48" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AF10" s="49" t="s">
+        <v>32</v>
+      </c>
+      <c r="AG10" s="50" t="s">
+        <v>30</v>
+      </c>
+      <c r="AH10" s="51" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI10" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="AG10" s="50" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH10" s="51" t="s">
-        <v>32</v>
-      </c>
-      <c r="AI10" s="49" t="s">
+      <c r="AJ10" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="AJ10" s="50" t="s">
+      <c r="AK10" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="AK10" s="52" t="s">
-        <v>36</v>
-      </c>
       <c r="AL10" s="53" t="s">
+        <v>92</v>
+      </c>
+      <c r="AM10" s="44" t="s">
         <v>93</v>
-      </c>
-      <c r="AM10" s="44" t="s">
-        <v>94</v>
       </c>
       <c r="AN10" s="54">
         <v>7</v>
       </c>
       <c r="AO10" s="55" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AP10" s="47" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AQ10" s="55">
         <v>8</v>
       </c>
       <c r="AR10" s="44" t="s">
+        <v>45</v>
+      </c>
+      <c r="AS10" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="AS10" s="44" t="s">
+      <c r="AT10" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="AT10" s="44" t="s">
+      <c r="AU10" s="56" t="s">
         <v>48</v>
       </c>
-      <c r="AU10" s="56" t="s">
+      <c r="AV10" s="56" t="s">
         <v>49</v>
       </c>
-      <c r="AV10" s="56" t="s">
+      <c r="AW10" s="56" t="s">
         <v>50</v>
       </c>
-      <c r="AW10" s="56" t="s">
-        <v>51</v>
-      </c>
       <c r="AX10" s="56" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AY10" s="56">
         <v>125</v>
@@ -3723,16 +3752,16 @@
         <v>125</v>
       </c>
       <c r="BA10" s="56" t="s">
+        <v>62</v>
+      </c>
+      <c r="BB10" s="56" t="s">
         <v>63</v>
       </c>
-      <c r="BB10" s="56" t="s">
+      <c r="BC10" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="BD10" s="56" t="s">
         <v>64</v>
-      </c>
-      <c r="BC10" s="56" t="s">
-        <v>66</v>
-      </c>
-      <c r="BD10" s="56" t="s">
-        <v>65</v>
       </c>
       <c r="BE10" s="64">
         <v>41309</v>
@@ -3744,17 +3773,19 @@
         <v>16.780833000000001</v>
       </c>
       <c r="BH10" s="44" t="s">
+        <v>102</v>
+      </c>
+      <c r="BI10" s="44" t="s">
         <v>103</v>
       </c>
-      <c r="BI10" s="44" t="s">
-        <v>104</v>
-      </c>
-      <c r="BJ10" s="44"/>
+      <c r="BJ10" s="44" t="s">
+        <v>143</v>
+      </c>
       <c r="BK10" s="56" t="s">
+        <v>60</v>
+      </c>
+      <c r="BL10" s="68" t="s">
         <v>61</v>
-      </c>
-      <c r="BL10" s="68" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:64" ht="16" thickTop="1"/>

</xml_diff>